<commit_message>
Fixed algo 7 bug + added NOTCON case for uww/agg scheme
</commit_message>
<xml_diff>
--- a/uwwtd website/sites/all/modules/uwwtd/model/2015_register_model_20160125_1.xlsx
+++ b/uwwtd website/sites/all/modules/uwwtd/model/2015_register_model_20160125_1.xlsx
@@ -4899,9 +4899,6 @@
     <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="29" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -4972,6 +4969,48 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="7" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="8" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="11" fillId="6" borderId="6" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="59" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="11" fillId="7" borderId="6" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="11" fillId="7" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
     </xf>
@@ -5006,9 +5045,6 @@
     <xf numFmtId="3" fontId="11" fillId="6" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -5057,44 +5093,92 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="7" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="32" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="32" fillId="11" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="4" borderId="7" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="16" borderId="7" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="16" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="8" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="12" fillId="11" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="12" fillId="19" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="11" fillId="6" borderId="6" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="59" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="11" fillId="7" borderId="6" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="11" fillId="7" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="14" fontId="32" fillId="22" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="32" fillId="22" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="32" fillId="22" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="32" fillId="11" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="29" fillId="20" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="12" fillId="11" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="12" fillId="11" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="32" fillId="12" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -5102,97 +5186,22 @@
     <xf numFmtId="3" fontId="32" fillId="12" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="32" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="32" fillId="11" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="3" fontId="32" fillId="12" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="32" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="29" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="30" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="32" fillId="22" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="32" fillId="22" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="32" fillId="22" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="32" fillId="11" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="29" fillId="20" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="12" fillId="11" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="12" fillId="19" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="12" fillId="11" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="4" borderId="7" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="16" borderId="7" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="16" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="12" fillId="11" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="30" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="50" fillId="29" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5204,23 +5213,11 @@
     <xf numFmtId="0" fontId="62" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="30" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="30" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="50" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="50" fillId="29" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="29" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="168" fontId="64" fillId="31" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -5320,6 +5317,42 @@
     <xf numFmtId="3" fontId="12" fillId="11" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="3"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="60" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="38" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="19" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -5345,41 +5378,8 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="60" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="38" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="15">
@@ -5781,11 +5781,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="206812792"/>
-        <c:axId val="206813576"/>
+        <c:axId val="275934176"/>
+        <c:axId val="275931824"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="206812792"/>
+        <c:axId val="275934176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5883,7 +5883,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="206813576"/>
+        <c:crossAx val="275931824"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5891,7 +5891,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="206813576"/>
+        <c:axId val="275931824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6010,7 +6010,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="206812792"/>
+        <c:crossAx val="275934176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6145,7 +6145,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6397,11 +6396,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="254125680"/>
-        <c:axId val="254126072"/>
+        <c:axId val="284967128"/>
+        <c:axId val="284967520"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="254125680"/>
+        <c:axId val="284967128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6433,7 +6432,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -6500,7 +6498,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="254126072"/>
+        <c:crossAx val="284967520"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6508,7 +6506,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="254126072"/>
+        <c:axId val="284967520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -6628,7 +6626,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="254125680"/>
+        <c:crossAx val="284967128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7505,11 +7503,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="254127640"/>
-        <c:axId val="254128032"/>
+        <c:axId val="284969088"/>
+        <c:axId val="284969480"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="254127640"/>
+        <c:axId val="284969088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7613,7 +7611,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="254128032"/>
+        <c:crossAx val="284969480"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7621,7 +7619,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="254128032"/>
+        <c:axId val="284969480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7672,7 +7670,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="254127640"/>
+        <c:crossAx val="284969088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8038,11 +8036,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="254128816"/>
-        <c:axId val="251637368"/>
+        <c:axId val="284970264"/>
+        <c:axId val="276239032"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="254128816"/>
+        <c:axId val="284970264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8153,7 +8151,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="251637368"/>
+        <c:crossAx val="276239032"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8161,7 +8159,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="251637368"/>
+        <c:axId val="276239032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8268,7 +8266,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="254128816"/>
+        <c:crossAx val="284970264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8639,11 +8637,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="251638152"/>
-        <c:axId val="251638544"/>
+        <c:axId val="276239816"/>
+        <c:axId val="276240208"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="251638152"/>
+        <c:axId val="276239816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8754,7 +8752,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="251638544"/>
+        <c:crossAx val="276240208"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8762,7 +8760,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="251638544"/>
+        <c:axId val="276240208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8876,7 +8874,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="251638152"/>
+        <c:crossAx val="276239816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9357,11 +9355,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="251639328"/>
-        <c:axId val="251639720"/>
+        <c:axId val="276240992"/>
+        <c:axId val="276241384"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="251639328"/>
+        <c:axId val="276240992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9467,7 +9465,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="251639720"/>
+        <c:crossAx val="276241384"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9475,7 +9473,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="251639720"/>
+        <c:axId val="276241384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9597,7 +9595,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="251639328"/>
+        <c:crossAx val="276240992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9934,11 +9932,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="251640504"/>
-        <c:axId val="251640896"/>
+        <c:axId val="276242168"/>
+        <c:axId val="276242560"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="251640504"/>
+        <c:axId val="276242168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10049,7 +10047,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="251640896"/>
+        <c:crossAx val="276242560"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10057,7 +10055,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="251640896"/>
+        <c:axId val="276242560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10171,7 +10169,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="251640504"/>
+        <c:crossAx val="276242168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10508,11 +10506,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="251756096"/>
-        <c:axId val="251756488"/>
+        <c:axId val="276243344"/>
+        <c:axId val="276243736"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="251756096"/>
+        <c:axId val="276243344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10623,7 +10621,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="251756488"/>
+        <c:crossAx val="276243736"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10631,7 +10629,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="251756488"/>
+        <c:axId val="276243736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10745,7 +10743,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="251756096"/>
+        <c:crossAx val="276243344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10880,7 +10878,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -11127,11 +11124,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="251757272"/>
-        <c:axId val="251757664"/>
+        <c:axId val="276244520"/>
+        <c:axId val="276244912"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="251757272"/>
+        <c:axId val="276244520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11163,7 +11160,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -11230,7 +11226,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="251757664"/>
+        <c:crossAx val="276244912"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11238,7 +11234,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="251757664"/>
+        <c:axId val="276244912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11357,7 +11353,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="251757272"/>
+        <c:crossAx val="276244520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11706,11 +11702,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="206814360"/>
-        <c:axId val="248872440"/>
+        <c:axId val="275933392"/>
+        <c:axId val="275934568"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="206814360"/>
+        <c:axId val="275933392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11808,7 +11804,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="248872440"/>
+        <c:crossAx val="275934568"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11816,7 +11812,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="248872440"/>
+        <c:axId val="275934568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11935,7 +11931,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="206814360"/>
+        <c:crossAx val="275933392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -13012,11 +13008,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="251320920"/>
-        <c:axId val="251321312"/>
+        <c:axId val="275936136"/>
+        <c:axId val="275936528"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="251320920"/>
+        <c:axId val="275936136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13114,7 +13110,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="251321312"/>
+        <c:crossAx val="275936528"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13122,7 +13118,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="251321312"/>
+        <c:axId val="275936528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13228,7 +13224,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="251320920"/>
+        <c:crossAx val="275936136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -13663,11 +13659,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="251322096"/>
-        <c:axId val="251322488"/>
+        <c:axId val="275937312"/>
+        <c:axId val="275937704"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="251322096"/>
+        <c:axId val="275937312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13765,7 +13761,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="251322488"/>
+        <c:crossAx val="275937704"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13773,7 +13769,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="251322488"/>
+        <c:axId val="275937704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13892,7 +13888,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="251322096"/>
+        <c:crossAx val="275937312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -14322,11 +14318,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="251323272"/>
-        <c:axId val="251323664"/>
+        <c:axId val="275938488"/>
+        <c:axId val="198458944"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="251323272"/>
+        <c:axId val="275938488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14424,7 +14420,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="251323664"/>
+        <c:crossAx val="198458944"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -14432,7 +14428,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="251323664"/>
+        <c:axId val="198458944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14551,7 +14547,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="251323272"/>
+        <c:crossAx val="275938488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -14686,7 +14682,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -15082,11 +15077,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="254051952"/>
-        <c:axId val="254052344"/>
+        <c:axId val="284963208"/>
+        <c:axId val="284963600"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="254051952"/>
+        <c:axId val="284963208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15129,7 +15124,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="254052344"/>
+        <c:crossAx val="284963600"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -15137,7 +15132,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="254052344"/>
+        <c:axId val="284963600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15188,7 +15183,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -15249,7 +15243,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="254051952"/>
+        <c:crossAx val="284963208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -15758,11 +15752,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="254053128"/>
-        <c:axId val="254053520"/>
+        <c:axId val="284964384"/>
+        <c:axId val="284964776"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="254053128"/>
+        <c:axId val="284964384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15805,7 +15799,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="254053520"/>
+        <c:crossAx val="284964776"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -15813,7 +15807,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="254053520"/>
+        <c:axId val="284964776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15924,7 +15918,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="254053128"/>
+        <c:crossAx val="284964384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -16018,7 +16012,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -16265,11 +16258,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="254054696"/>
-        <c:axId val="254055088"/>
+        <c:axId val="284965952"/>
+        <c:axId val="284966344"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="254054696"/>
+        <c:axId val="284965952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16298,7 +16291,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -16365,7 +16357,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="254055088"/>
+        <c:crossAx val="284966344"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -16373,7 +16365,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="254055088"/>
+        <c:axId val="284966344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -16493,7 +16485,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="254054696"/>
+        <c:crossAx val="284965952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -27394,54 +27386,54 @@
       <c r="AR3" s="5"/>
     </row>
     <row r="4" spans="1:44" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="597" t="s">
+      <c r="A4" s="596" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="598"/>
-      <c r="C4" s="598"/>
-      <c r="D4" s="598"/>
-      <c r="E4" s="599"/>
-      <c r="F4" s="599"/>
-      <c r="G4" s="599"/>
-      <c r="H4" s="599"/>
-      <c r="I4" s="599"/>
-      <c r="J4" s="599"/>
-      <c r="K4" s="599"/>
-      <c r="L4" s="599"/>
-      <c r="M4" s="599"/>
-      <c r="N4" s="599"/>
-      <c r="O4" s="599"/>
-      <c r="P4" s="599"/>
-      <c r="Q4" s="599"/>
-      <c r="R4" s="599"/>
-      <c r="S4" s="599"/>
-      <c r="T4" s="599"/>
-      <c r="U4" s="599"/>
-      <c r="V4" s="599"/>
-      <c r="W4" s="599"/>
-      <c r="X4" s="599"/>
-      <c r="Y4" s="599"/>
-      <c r="Z4" s="599"/>
-      <c r="AA4" s="599"/>
-      <c r="AB4" s="599"/>
-      <c r="AC4" s="599"/>
-      <c r="AD4" s="599"/>
-      <c r="AE4" s="599"/>
-      <c r="AF4" s="599"/>
-      <c r="AG4" s="599"/>
-      <c r="AH4" s="599"/>
-      <c r="AI4" s="599"/>
-      <c r="AJ4" s="599"/>
-      <c r="AK4" s="599"/>
-      <c r="AL4" s="599"/>
-      <c r="AM4" s="599"/>
-      <c r="AN4" s="599"/>
-      <c r="AO4" s="599"/>
-      <c r="AP4" s="599"/>
-      <c r="AQ4" s="600" t="s">
+      <c r="B4" s="597"/>
+      <c r="C4" s="597"/>
+      <c r="D4" s="597"/>
+      <c r="E4" s="598"/>
+      <c r="F4" s="598"/>
+      <c r="G4" s="598"/>
+      <c r="H4" s="598"/>
+      <c r="I4" s="598"/>
+      <c r="J4" s="598"/>
+      <c r="K4" s="598"/>
+      <c r="L4" s="598"/>
+      <c r="M4" s="598"/>
+      <c r="N4" s="598"/>
+      <c r="O4" s="598"/>
+      <c r="P4" s="598"/>
+      <c r="Q4" s="598"/>
+      <c r="R4" s="598"/>
+      <c r="S4" s="598"/>
+      <c r="T4" s="598"/>
+      <c r="U4" s="598"/>
+      <c r="V4" s="598"/>
+      <c r="W4" s="598"/>
+      <c r="X4" s="598"/>
+      <c r="Y4" s="598"/>
+      <c r="Z4" s="598"/>
+      <c r="AA4" s="598"/>
+      <c r="AB4" s="598"/>
+      <c r="AC4" s="598"/>
+      <c r="AD4" s="598"/>
+      <c r="AE4" s="598"/>
+      <c r="AF4" s="598"/>
+      <c r="AG4" s="598"/>
+      <c r="AH4" s="598"/>
+      <c r="AI4" s="598"/>
+      <c r="AJ4" s="598"/>
+      <c r="AK4" s="598"/>
+      <c r="AL4" s="598"/>
+      <c r="AM4" s="598"/>
+      <c r="AN4" s="598"/>
+      <c r="AO4" s="598"/>
+      <c r="AP4" s="598"/>
+      <c r="AQ4" s="599" t="s">
         <v>3</v>
       </c>
-      <c r="AR4" s="600"/>
+      <c r="AR4" s="599"/>
     </row>
     <row r="5" spans="1:44" ht="135" x14ac:dyDescent="0.25">
       <c r="A5" s="458" t="s">
@@ -27790,8 +27782,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:AF178"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A145" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E153" sqref="E153"/>
+    <sheetView tabSelected="1" topLeftCell="A154" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D159" sqref="D159:D162"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27814,20 +27806,20 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A3" s="734" t="s">
+      <c r="A3" s="724" t="s">
         <v>349</v>
       </c>
-      <c r="B3" s="736" t="s">
+      <c r="B3" s="726" t="s">
         <v>350</v>
       </c>
-      <c r="C3" s="737"/>
-      <c r="D3" s="732" t="s">
+      <c r="C3" s="727"/>
+      <c r="D3" s="722" t="s">
         <v>359</v>
       </c>
-      <c r="E3" s="733"/>
+      <c r="E3" s="723"/>
     </row>
     <row r="4" spans="1:28" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A4" s="735"/>
+      <c r="A4" s="725"/>
       <c r="B4" s="473" t="s">
         <v>224</v>
       </c>
@@ -27851,13 +27843,13 @@
       </c>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A5" s="566" t="s">
+      <c r="A5" s="565" t="s">
         <v>352</v>
       </c>
-      <c r="B5" s="567"/>
-      <c r="C5" s="568"/>
-      <c r="D5" s="569"/>
-      <c r="E5" s="570"/>
+      <c r="B5" s="566"/>
+      <c r="C5" s="567"/>
+      <c r="D5" s="568"/>
+      <c r="E5" s="569"/>
       <c r="Z5" t="str">
         <f>A5</f>
         <v>2000-10000</v>
@@ -27872,13 +27864,13 @@
       </c>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A6" s="571" t="s">
+      <c r="A6" s="570" t="s">
         <v>461</v>
       </c>
-      <c r="B6" s="572"/>
-      <c r="C6" s="573"/>
-      <c r="D6" s="571"/>
-      <c r="E6" s="574"/>
+      <c r="B6" s="571"/>
+      <c r="C6" s="572"/>
+      <c r="D6" s="570"/>
+      <c r="E6" s="573"/>
       <c r="Z6" t="str">
         <f>A6</f>
         <v>10001-15000</v>
@@ -27893,13 +27885,13 @@
       </c>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A7" s="571" t="s">
+      <c r="A7" s="570" t="s">
         <v>462</v>
       </c>
-      <c r="B7" s="572"/>
-      <c r="C7" s="573"/>
-      <c r="D7" s="571"/>
-      <c r="E7" s="574"/>
+      <c r="B7" s="571"/>
+      <c r="C7" s="572"/>
+      <c r="D7" s="570"/>
+      <c r="E7" s="573"/>
       <c r="Z7" t="str">
         <f>A7</f>
         <v>15001-100000</v>
@@ -27914,13 +27906,13 @@
       </c>
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A8" s="571" t="s">
+      <c r="A8" s="570" t="s">
         <v>463</v>
       </c>
-      <c r="B8" s="572"/>
-      <c r="C8" s="573"/>
-      <c r="D8" s="571"/>
-      <c r="E8" s="574"/>
+      <c r="B8" s="571"/>
+      <c r="C8" s="572"/>
+      <c r="D8" s="570"/>
+      <c r="E8" s="573"/>
       <c r="Z8" t="str">
         <f t="shared" ref="Z8:Z9" si="0">A8</f>
         <v>100001-150000</v>
@@ -27935,13 +27927,13 @@
       </c>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A9" s="571" t="s">
+      <c r="A9" s="570" t="s">
         <v>464</v>
       </c>
-      <c r="B9" s="572"/>
-      <c r="C9" s="573"/>
-      <c r="D9" s="571"/>
-      <c r="E9" s="574"/>
+      <c r="B9" s="571"/>
+      <c r="C9" s="572"/>
+      <c r="D9" s="570"/>
+      <c r="E9" s="573"/>
       <c r="Z9" t="str">
         <f t="shared" si="0"/>
         <v>&gt;150000</v>
@@ -27981,7 +27973,7 @@
       </c>
     </row>
     <row r="13" spans="1:28" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="734" t="s">
+      <c r="A13" s="724" t="s">
         <v>353</v>
       </c>
       <c r="B13" s="472" t="s">
@@ -28004,7 +27996,7 @@
       </c>
     </row>
     <row r="14" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A14" s="735"/>
+      <c r="A14" s="725"/>
       <c r="B14" s="475" t="s">
         <v>354</v>
       </c>
@@ -28087,10 +28079,10 @@
       <c r="A22" s="478" t="s">
         <v>313</v>
       </c>
-      <c r="B22" s="738" t="s">
+      <c r="B22" s="728" t="s">
         <v>350</v>
       </c>
-      <c r="C22" s="739"/>
+      <c r="C22" s="729"/>
     </row>
     <row r="23" spans="1:30" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="479"/>
@@ -28114,11 +28106,11 @@
       </c>
     </row>
     <row r="24" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A24" s="561" t="s">
+      <c r="A24" s="560" t="s">
         <v>316</v>
       </c>
-      <c r="B24" s="562"/>
-      <c r="C24" s="562"/>
+      <c r="B24" s="561"/>
+      <c r="C24" s="561"/>
       <c r="Z24" t="str">
         <f>A25</f>
         <v xml:space="preserve">discharged into surface waters: Pipelines </v>
@@ -28137,11 +28129,11 @@
       </c>
     </row>
     <row r="25" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A25" s="575" t="s">
+      <c r="A25" s="574" t="s">
         <v>465</v>
       </c>
-      <c r="B25" s="576"/>
-      <c r="C25" s="577"/>
+      <c r="B25" s="575"/>
+      <c r="C25" s="576"/>
       <c r="Z25" t="str">
         <f t="shared" ref="Z25:Z31" si="5">A26</f>
         <v xml:space="preserve">discharged into surface waters: Ships </v>
@@ -28160,11 +28152,11 @@
       </c>
     </row>
     <row r="26" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A26" s="575" t="s">
+      <c r="A26" s="574" t="s">
         <v>466</v>
       </c>
-      <c r="B26" s="576"/>
-      <c r="C26" s="577"/>
+      <c r="B26" s="575"/>
+      <c r="C26" s="576"/>
       <c r="Z26" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve">discharged into surface waters: Others </v>
@@ -28183,11 +28175,11 @@
       </c>
     </row>
     <row r="27" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A27" s="575" t="s">
+      <c r="A27" s="574" t="s">
         <v>467</v>
       </c>
-      <c r="B27" s="576"/>
-      <c r="C27" s="577"/>
+      <c r="B27" s="575"/>
+      <c r="C27" s="576"/>
       <c r="Z27" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve">re-used: Soil and agriculture </v>
@@ -28206,11 +28198,11 @@
       </c>
     </row>
     <row r="28" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A28" s="563" t="s">
+      <c r="A28" s="562" t="s">
         <v>361</v>
       </c>
-      <c r="B28" s="562"/>
-      <c r="C28" s="562"/>
+      <c r="B28" s="561"/>
+      <c r="C28" s="561"/>
       <c r="Z28" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve">re-used: Others </v>
@@ -28229,11 +28221,11 @@
       </c>
     </row>
     <row r="29" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A29" s="563" t="s">
+      <c r="A29" s="562" t="s">
         <v>362</v>
       </c>
-      <c r="B29" s="564"/>
-      <c r="C29" s="564"/>
+      <c r="B29" s="563"/>
+      <c r="C29" s="563"/>
       <c r="Z29" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve">disposed: Landfill </v>
@@ -28252,11 +28244,11 @@
       </c>
     </row>
     <row r="30" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A30" s="563" t="s">
+      <c r="A30" s="562" t="s">
         <v>456</v>
       </c>
-      <c r="B30" s="564"/>
-      <c r="C30" s="564"/>
+      <c r="B30" s="563"/>
+      <c r="C30" s="563"/>
       <c r="Z30" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve">disposed: Incineration </v>
@@ -28275,11 +28267,11 @@
       </c>
     </row>
     <row r="31" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A31" s="563" t="s">
+      <c r="A31" s="562" t="s">
         <v>363</v>
       </c>
-      <c r="B31" s="564"/>
-      <c r="C31" s="564"/>
+      <c r="B31" s="563"/>
+      <c r="C31" s="563"/>
       <c r="Z31" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve">disposed: Others </v>
@@ -28298,11 +28290,11 @@
       </c>
     </row>
     <row r="32" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A32" s="563" t="s">
+      <c r="A32" s="562" t="s">
         <v>364</v>
       </c>
-      <c r="B32" s="564"/>
-      <c r="C32" s="564"/>
+      <c r="B32" s="563"/>
+      <c r="C32" s="563"/>
     </row>
     <row r="35" spans="1:32" ht="33" x14ac:dyDescent="0.35">
       <c r="A35" s="483" t="s">
@@ -28342,14 +28334,14 @@
       <c r="A41" s="481" t="s">
         <v>365</v>
       </c>
-      <c r="B41" s="728" t="s">
+      <c r="B41" s="718" t="s">
         <v>350</v>
       </c>
-      <c r="C41" s="729"/>
-      <c r="D41" s="730" t="s">
+      <c r="C41" s="719"/>
+      <c r="D41" s="720" t="s">
         <v>359</v>
       </c>
-      <c r="E41" s="731"/>
+      <c r="E41" s="721"/>
       <c r="AA41" t="s">
         <v>442</v>
       </c>
@@ -28412,13 +28404,13 @@
       </c>
     </row>
     <row r="43" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A43" s="569" t="s">
+      <c r="A43" s="568" t="s">
         <v>368</v>
       </c>
-      <c r="B43" s="578"/>
-      <c r="C43" s="578"/>
-      <c r="D43" s="578"/>
-      <c r="E43" s="578"/>
+      <c r="B43" s="577"/>
+      <c r="C43" s="577"/>
+      <c r="D43" s="577"/>
+      <c r="E43" s="577"/>
       <c r="Z43" t="s">
         <v>378</v>
       </c>
@@ -28448,76 +28440,76 @@
       </c>
     </row>
     <row r="44" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A44" s="569" t="s">
+      <c r="A44" s="568" t="s">
         <v>369</v>
       </c>
-      <c r="B44" s="578"/>
-      <c r="C44" s="578"/>
-      <c r="D44" s="578"/>
-      <c r="E44" s="578"/>
+      <c r="B44" s="577"/>
+      <c r="C44" s="577"/>
+      <c r="D44" s="577"/>
+      <c r="E44" s="577"/>
     </row>
     <row r="45" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A45" s="569" t="s">
+      <c r="A45" s="568" t="s">
         <v>458</v>
       </c>
-      <c r="B45" s="578"/>
-      <c r="C45" s="578"/>
-      <c r="D45" s="578"/>
-      <c r="E45" s="578"/>
+      <c r="B45" s="577"/>
+      <c r="C45" s="577"/>
+      <c r="D45" s="577"/>
+      <c r="E45" s="577"/>
     </row>
     <row r="46" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A46" s="569" t="s">
+      <c r="A46" s="568" t="s">
         <v>370</v>
       </c>
-      <c r="B46" s="578"/>
-      <c r="C46" s="578"/>
-      <c r="D46" s="578"/>
-      <c r="E46" s="578"/>
+      <c r="B46" s="577"/>
+      <c r="C46" s="577"/>
+      <c r="D46" s="577"/>
+      <c r="E46" s="577"/>
     </row>
     <row r="47" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A47" s="569" t="s">
+      <c r="A47" s="568" t="s">
         <v>371</v>
       </c>
-      <c r="B47" s="578"/>
-      <c r="C47" s="578"/>
-      <c r="D47" s="578"/>
-      <c r="E47" s="578"/>
+      <c r="B47" s="577"/>
+      <c r="C47" s="577"/>
+      <c r="D47" s="577"/>
+      <c r="E47" s="577"/>
     </row>
     <row r="48" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A48" s="569" t="s">
+      <c r="A48" s="568" t="s">
         <v>459</v>
       </c>
-      <c r="B48" s="578"/>
-      <c r="C48" s="578"/>
-      <c r="D48" s="578"/>
-      <c r="E48" s="578"/>
+      <c r="B48" s="577"/>
+      <c r="C48" s="577"/>
+      <c r="D48" s="577"/>
+      <c r="E48" s="577"/>
     </row>
     <row r="49" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A49" s="569" t="s">
+      <c r="A49" s="568" t="s">
         <v>372</v>
       </c>
-      <c r="B49" s="578"/>
-      <c r="C49" s="578"/>
-      <c r="D49" s="578"/>
-      <c r="E49" s="578"/>
+      <c r="B49" s="577"/>
+      <c r="C49" s="577"/>
+      <c r="D49" s="577"/>
+      <c r="E49" s="577"/>
     </row>
     <row r="50" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A50" s="569" t="s">
+      <c r="A50" s="568" t="s">
         <v>373</v>
       </c>
-      <c r="B50" s="578"/>
-      <c r="C50" s="578"/>
-      <c r="D50" s="578"/>
-      <c r="E50" s="578"/>
+      <c r="B50" s="577"/>
+      <c r="C50" s="577"/>
+      <c r="D50" s="577"/>
+      <c r="E50" s="577"/>
     </row>
     <row r="51" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A51" s="569" t="s">
+      <c r="A51" s="568" t="s">
         <v>460</v>
       </c>
-      <c r="B51" s="578"/>
-      <c r="C51" s="578"/>
-      <c r="D51" s="578"/>
-      <c r="E51" s="578"/>
+      <c r="B51" s="577"/>
+      <c r="C51" s="577"/>
+      <c r="D51" s="577"/>
+      <c r="E51" s="577"/>
     </row>
     <row r="52" spans="1:30" x14ac:dyDescent="0.25">
       <c r="AB52" s="551" t="s">
@@ -28532,22 +28524,22 @@
     </row>
     <row r="53" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A53" s="489"/>
-      <c r="B53" s="579" t="s">
+      <c r="B53" s="578" t="s">
         <v>377</v>
       </c>
-      <c r="C53" s="579" t="s">
+      <c r="C53" s="578" t="s">
         <v>378</v>
       </c>
-      <c r="D53" s="579" t="s">
+      <c r="D53" s="578" t="s">
         <v>457</v>
       </c>
-      <c r="E53" s="579" t="s">
+      <c r="E53" s="578" t="s">
         <v>377</v>
       </c>
-      <c r="F53" s="579" t="s">
+      <c r="F53" s="578" t="s">
         <v>378</v>
       </c>
-      <c r="G53" s="579" t="s">
+      <c r="G53" s="578" t="s">
         <v>457</v>
       </c>
       <c r="AA53" t="s">
@@ -28570,12 +28562,12 @@
       <c r="A54" s="491" t="s">
         <v>379</v>
       </c>
-      <c r="B54" s="578"/>
-      <c r="C54" s="578"/>
-      <c r="D54" s="578"/>
-      <c r="E54" s="569"/>
-      <c r="F54" s="569"/>
-      <c r="G54" s="578"/>
+      <c r="B54" s="577"/>
+      <c r="C54" s="577"/>
+      <c r="D54" s="577"/>
+      <c r="E54" s="568"/>
+      <c r="F54" s="568"/>
+      <c r="G54" s="577"/>
       <c r="AA54" t="s">
         <v>449</v>
       </c>
@@ -28596,12 +28588,12 @@
       <c r="A55" s="491" t="s">
         <v>384</v>
       </c>
-      <c r="B55" s="569"/>
-      <c r="C55" s="569"/>
-      <c r="D55" s="569"/>
-      <c r="E55" s="578"/>
-      <c r="F55" s="578"/>
-      <c r="G55" s="578"/>
+      <c r="B55" s="568"/>
+      <c r="C55" s="568"/>
+      <c r="D55" s="568"/>
+      <c r="E55" s="577"/>
+      <c r="F55" s="577"/>
+      <c r="G55" s="577"/>
       <c r="AA55" t="s">
         <v>450</v>
       </c>
@@ -28620,12 +28612,12 @@
     </row>
     <row r="56" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A56" s="491"/>
-      <c r="B56" s="578"/>
-      <c r="C56" s="578"/>
-      <c r="D56" s="578"/>
-      <c r="E56" s="578"/>
-      <c r="F56" s="578"/>
-      <c r="G56" s="578"/>
+      <c r="B56" s="577"/>
+      <c r="C56" s="577"/>
+      <c r="D56" s="577"/>
+      <c r="E56" s="577"/>
+      <c r="F56" s="577"/>
+      <c r="G56" s="577"/>
       <c r="AA56" t="s">
         <v>451</v>
       </c>
@@ -28646,12 +28638,12 @@
       <c r="A57" s="491" t="s">
         <v>380</v>
       </c>
-      <c r="B57" s="578"/>
-      <c r="C57" s="578"/>
-      <c r="D57" s="578"/>
-      <c r="E57" s="569"/>
-      <c r="F57" s="569"/>
-      <c r="G57" s="578"/>
+      <c r="B57" s="577"/>
+      <c r="C57" s="577"/>
+      <c r="D57" s="577"/>
+      <c r="E57" s="568"/>
+      <c r="F57" s="568"/>
+      <c r="G57" s="577"/>
       <c r="AA57" t="s">
         <v>452</v>
       </c>
@@ -28672,12 +28664,12 @@
       <c r="A58" s="491" t="s">
         <v>383</v>
       </c>
-      <c r="B58" s="569"/>
-      <c r="C58" s="569"/>
-      <c r="D58" s="569"/>
-      <c r="E58" s="578"/>
-      <c r="F58" s="578"/>
-      <c r="G58" s="578"/>
+      <c r="B58" s="568"/>
+      <c r="C58" s="568"/>
+      <c r="D58" s="568"/>
+      <c r="E58" s="577"/>
+      <c r="F58" s="577"/>
+      <c r="G58" s="577"/>
       <c r="AA58" t="s">
         <v>453</v>
       </c>
@@ -28696,41 +28688,41 @@
     </row>
     <row r="59" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A59" s="491"/>
-      <c r="B59" s="578"/>
-      <c r="C59" s="578"/>
-      <c r="D59" s="578"/>
-      <c r="E59" s="578"/>
-      <c r="F59" s="578"/>
-      <c r="G59" s="578"/>
+      <c r="B59" s="577"/>
+      <c r="C59" s="577"/>
+      <c r="D59" s="577"/>
+      <c r="E59" s="577"/>
+      <c r="F59" s="577"/>
+      <c r="G59" s="577"/>
     </row>
     <row r="60" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A60" s="491" t="s">
         <v>381</v>
       </c>
-      <c r="B60" s="578"/>
-      <c r="C60" s="578"/>
-      <c r="D60" s="578"/>
-      <c r="E60" s="569"/>
-      <c r="F60" s="569"/>
-      <c r="G60" s="578"/>
+      <c r="B60" s="577"/>
+      <c r="C60" s="577"/>
+      <c r="D60" s="577"/>
+      <c r="E60" s="568"/>
+      <c r="F60" s="568"/>
+      <c r="G60" s="577"/>
     </row>
     <row r="61" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A61" s="491" t="s">
         <v>382</v>
       </c>
-      <c r="B61" s="569"/>
-      <c r="C61" s="569"/>
-      <c r="D61" s="569"/>
-      <c r="E61" s="578"/>
-      <c r="F61" s="578"/>
-      <c r="G61" s="578"/>
+      <c r="B61" s="568"/>
+      <c r="C61" s="568"/>
+      <c r="D61" s="568"/>
+      <c r="E61" s="577"/>
+      <c r="F61" s="577"/>
+      <c r="G61" s="577"/>
     </row>
     <row r="62" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A62" s="492"/>
       <c r="B62" s="493"/>
       <c r="C62" s="493"/>
-      <c r="D62" s="560"/>
-      <c r="G62" s="560"/>
+      <c r="D62" s="559"/>
+      <c r="G62" s="559"/>
     </row>
     <row r="63" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A63" s="474"/>
@@ -28740,16 +28732,16 @@
       <c r="C63" s="494" t="s">
         <v>378</v>
       </c>
-      <c r="D63" s="579" t="s">
+      <c r="D63" s="578" t="s">
         <v>457</v>
       </c>
-      <c r="E63" s="581" t="s">
+      <c r="E63" s="580" t="s">
         <v>377</v>
       </c>
-      <c r="F63" s="581" t="s">
+      <c r="F63" s="580" t="s">
         <v>378</v>
       </c>
-      <c r="G63" s="579" t="s">
+      <c r="G63" s="578" t="s">
         <v>457</v>
       </c>
       <c r="AB63" s="552" t="s">
@@ -28766,12 +28758,12 @@
       <c r="A64" s="491" t="s">
         <v>379</v>
       </c>
-      <c r="B64" s="580"/>
-      <c r="C64" s="580"/>
-      <c r="D64" s="580"/>
-      <c r="E64" s="566"/>
-      <c r="F64" s="566"/>
-      <c r="G64" s="580"/>
+      <c r="B64" s="579"/>
+      <c r="C64" s="579"/>
+      <c r="D64" s="579"/>
+      <c r="E64" s="565"/>
+      <c r="F64" s="565"/>
+      <c r="G64" s="579"/>
       <c r="AA64" t="s">
         <v>448</v>
       </c>
@@ -28792,12 +28784,12 @@
       <c r="A65" s="491" t="s">
         <v>384</v>
       </c>
-      <c r="B65" s="566"/>
-      <c r="C65" s="566"/>
-      <c r="D65" s="566"/>
-      <c r="E65" s="580"/>
-      <c r="F65" s="580"/>
-      <c r="G65" s="580"/>
+      <c r="B65" s="565"/>
+      <c r="C65" s="565"/>
+      <c r="D65" s="565"/>
+      <c r="E65" s="579"/>
+      <c r="F65" s="579"/>
+      <c r="G65" s="579"/>
       <c r="AA65" t="s">
         <v>449</v>
       </c>
@@ -28816,12 +28808,12 @@
     </row>
     <row r="66" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A66" s="491"/>
-      <c r="B66" s="580"/>
-      <c r="C66" s="580"/>
-      <c r="D66" s="580"/>
-      <c r="E66" s="580"/>
-      <c r="F66" s="580"/>
-      <c r="G66" s="580"/>
+      <c r="B66" s="579"/>
+      <c r="C66" s="579"/>
+      <c r="D66" s="579"/>
+      <c r="E66" s="579"/>
+      <c r="F66" s="579"/>
+      <c r="G66" s="579"/>
       <c r="AA66" t="s">
         <v>450</v>
       </c>
@@ -28842,12 +28834,12 @@
       <c r="A67" s="491" t="s">
         <v>380</v>
       </c>
-      <c r="B67" s="580"/>
-      <c r="C67" s="580"/>
-      <c r="D67" s="580"/>
-      <c r="E67" s="566"/>
-      <c r="F67" s="566"/>
-      <c r="G67" s="580"/>
+      <c r="B67" s="579"/>
+      <c r="C67" s="579"/>
+      <c r="D67" s="579"/>
+      <c r="E67" s="565"/>
+      <c r="F67" s="565"/>
+      <c r="G67" s="579"/>
       <c r="AA67" t="s">
         <v>451</v>
       </c>
@@ -28868,12 +28860,12 @@
       <c r="A68" s="491" t="s">
         <v>383</v>
       </c>
-      <c r="B68" s="566"/>
-      <c r="C68" s="566"/>
-      <c r="D68" s="566"/>
-      <c r="E68" s="580"/>
-      <c r="F68" s="580"/>
-      <c r="G68" s="580"/>
+      <c r="B68" s="565"/>
+      <c r="C68" s="565"/>
+      <c r="D68" s="565"/>
+      <c r="E68" s="579"/>
+      <c r="F68" s="579"/>
+      <c r="G68" s="579"/>
       <c r="AA68" t="s">
         <v>452</v>
       </c>
@@ -28892,12 +28884,12 @@
     </row>
     <row r="69" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A69" s="491"/>
-      <c r="B69" s="580"/>
-      <c r="C69" s="580"/>
-      <c r="D69" s="580"/>
-      <c r="E69" s="580"/>
-      <c r="F69" s="580"/>
-      <c r="G69" s="580"/>
+      <c r="B69" s="579"/>
+      <c r="C69" s="579"/>
+      <c r="D69" s="579"/>
+      <c r="E69" s="579"/>
+      <c r="F69" s="579"/>
+      <c r="G69" s="579"/>
       <c r="AA69" t="s">
         <v>453</v>
       </c>
@@ -28918,23 +28910,23 @@
       <c r="A70" s="491" t="s">
         <v>381</v>
       </c>
-      <c r="B70" s="580"/>
-      <c r="C70" s="580"/>
-      <c r="D70" s="580"/>
-      <c r="E70" s="566"/>
-      <c r="F70" s="566"/>
-      <c r="G70" s="580"/>
+      <c r="B70" s="579"/>
+      <c r="C70" s="579"/>
+      <c r="D70" s="579"/>
+      <c r="E70" s="565"/>
+      <c r="F70" s="565"/>
+      <c r="G70" s="579"/>
     </row>
     <row r="71" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A71" s="491" t="s">
         <v>382</v>
       </c>
-      <c r="B71" s="566"/>
-      <c r="C71" s="566"/>
-      <c r="D71" s="566"/>
-      <c r="E71" s="580"/>
-      <c r="F71" s="580"/>
-      <c r="G71" s="580"/>
+      <c r="B71" s="565"/>
+      <c r="C71" s="565"/>
+      <c r="D71" s="565"/>
+      <c r="E71" s="579"/>
+      <c r="F71" s="579"/>
+      <c r="G71" s="579"/>
     </row>
     <row r="73" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
@@ -29013,14 +29005,14 @@
       <c r="A77" s="522" t="s">
         <v>271</v>
       </c>
-      <c r="B77" s="586"/>
-      <c r="C77" s="586"/>
-      <c r="D77" s="586"/>
-      <c r="E77" s="586"/>
-      <c r="F77" s="587"/>
-      <c r="G77" s="587"/>
-      <c r="H77" s="587"/>
-      <c r="I77" s="587"/>
+      <c r="B77" s="585"/>
+      <c r="C77" s="585"/>
+      <c r="D77" s="585"/>
+      <c r="E77" s="585"/>
+      <c r="F77" s="586"/>
+      <c r="G77" s="586"/>
+      <c r="H77" s="586"/>
+      <c r="I77" s="586"/>
       <c r="Z77" t="s">
         <v>271</v>
       </c>
@@ -29048,14 +29040,14 @@
       <c r="A78" s="253" t="s">
         <v>260</v>
       </c>
-      <c r="B78" s="590"/>
-      <c r="C78" s="586"/>
-      <c r="D78" s="590"/>
-      <c r="E78" s="586"/>
-      <c r="F78" s="587"/>
-      <c r="G78" s="587"/>
-      <c r="H78" s="587"/>
-      <c r="I78" s="587"/>
+      <c r="B78" s="589"/>
+      <c r="C78" s="585"/>
+      <c r="D78" s="589"/>
+      <c r="E78" s="585"/>
+      <c r="F78" s="586"/>
+      <c r="G78" s="586"/>
+      <c r="H78" s="586"/>
+      <c r="I78" s="586"/>
       <c r="Z78" s="253" t="s">
         <v>260</v>
       </c>
@@ -29083,14 +29075,14 @@
       <c r="A79" s="253" t="s">
         <v>389</v>
       </c>
-      <c r="B79" s="590"/>
-      <c r="C79" s="586"/>
-      <c r="D79" s="590"/>
-      <c r="E79" s="586"/>
-      <c r="F79" s="587"/>
-      <c r="G79" s="587"/>
-      <c r="H79" s="587"/>
-      <c r="I79" s="587"/>
+      <c r="B79" s="589"/>
+      <c r="C79" s="585"/>
+      <c r="D79" s="589"/>
+      <c r="E79" s="585"/>
+      <c r="F79" s="586"/>
+      <c r="G79" s="586"/>
+      <c r="H79" s="586"/>
+      <c r="I79" s="586"/>
       <c r="Z79" s="253" t="s">
         <v>389</v>
       </c>
@@ -29118,14 +29110,14 @@
       <c r="A80" s="253" t="s">
         <v>390</v>
       </c>
-      <c r="B80" s="590"/>
-      <c r="C80" s="586"/>
-      <c r="D80" s="590"/>
-      <c r="E80" s="586"/>
-      <c r="F80" s="587"/>
-      <c r="G80" s="587"/>
-      <c r="H80" s="587"/>
-      <c r="I80" s="587"/>
+      <c r="B80" s="589"/>
+      <c r="C80" s="585"/>
+      <c r="D80" s="589"/>
+      <c r="E80" s="585"/>
+      <c r="F80" s="586"/>
+      <c r="G80" s="586"/>
+      <c r="H80" s="586"/>
+      <c r="I80" s="586"/>
       <c r="Z80" s="253" t="s">
         <v>390</v>
       </c>
@@ -29153,14 +29145,14 @@
       <c r="A81" s="253" t="s">
         <v>391</v>
       </c>
-      <c r="B81" s="591"/>
-      <c r="C81" s="586"/>
-      <c r="D81" s="591"/>
-      <c r="E81" s="586"/>
-      <c r="F81" s="588"/>
-      <c r="G81" s="589"/>
-      <c r="H81" s="588"/>
-      <c r="I81" s="589"/>
+      <c r="B81" s="590"/>
+      <c r="C81" s="585"/>
+      <c r="D81" s="590"/>
+      <c r="E81" s="585"/>
+      <c r="F81" s="587"/>
+      <c r="G81" s="588"/>
+      <c r="H81" s="587"/>
+      <c r="I81" s="588"/>
       <c r="Z81" s="253" t="s">
         <v>391</v>
       </c>
@@ -29188,14 +29180,14 @@
       <c r="A82" s="523" t="s">
         <v>392</v>
       </c>
-      <c r="B82" s="591"/>
-      <c r="C82" s="586"/>
-      <c r="D82" s="591"/>
-      <c r="E82" s="586"/>
-      <c r="F82" s="588"/>
-      <c r="G82" s="589"/>
-      <c r="H82" s="588"/>
-      <c r="I82" s="589"/>
+      <c r="B82" s="590"/>
+      <c r="C82" s="585"/>
+      <c r="D82" s="590"/>
+      <c r="E82" s="585"/>
+      <c r="F82" s="587"/>
+      <c r="G82" s="588"/>
+      <c r="H82" s="587"/>
+      <c r="I82" s="588"/>
       <c r="Z82" s="523" t="s">
         <v>392</v>
       </c>
@@ -29225,14 +29217,14 @@
       </c>
     </row>
     <row r="85" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="B85" s="721" t="s">
+      <c r="B85" s="732" t="s">
         <v>350</v>
       </c>
-      <c r="C85" s="722"/>
-      <c r="D85" s="721" t="s">
+      <c r="C85" s="733"/>
+      <c r="D85" s="732" t="s">
         <v>359</v>
       </c>
-      <c r="E85" s="722"/>
+      <c r="E85" s="733"/>
       <c r="Z85" t="s">
         <v>455</v>
       </c>
@@ -29245,14 +29237,14 @@
     </row>
     <row r="86" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A86" s="324"/>
-      <c r="B86" s="723" t="s">
+      <c r="B86" s="734" t="s">
         <v>258</v>
       </c>
-      <c r="C86" s="687"/>
-      <c r="D86" s="723" t="s">
+      <c r="C86" s="686"/>
+      <c r="D86" s="734" t="s">
         <v>258</v>
       </c>
-      <c r="E86" s="687"/>
+      <c r="E86" s="686"/>
       <c r="Z86" s="525" t="s">
         <v>259</v>
       </c>
@@ -29297,10 +29289,10 @@
       <c r="A88" s="525" t="s">
         <v>259</v>
       </c>
-      <c r="B88" s="592"/>
-      <c r="C88" s="582"/>
-      <c r="D88" s="592"/>
-      <c r="E88" s="582"/>
+      <c r="B88" s="591"/>
+      <c r="C88" s="581"/>
+      <c r="D88" s="591"/>
+      <c r="E88" s="581"/>
       <c r="Z88" s="525" t="s">
         <v>395</v>
       </c>
@@ -29317,10 +29309,10 @@
       <c r="A89" s="526" t="s">
         <v>394</v>
       </c>
-      <c r="B89" s="592"/>
-      <c r="C89" s="565"/>
-      <c r="D89" s="592"/>
-      <c r="E89" s="565"/>
+      <c r="B89" s="591"/>
+      <c r="C89" s="564"/>
+      <c r="D89" s="591"/>
+      <c r="E89" s="564"/>
       <c r="Z89" s="526" t="s">
         <v>396</v>
       </c>
@@ -29337,10 +29329,10 @@
       <c r="A90" s="525" t="s">
         <v>395</v>
       </c>
-      <c r="B90" s="592"/>
-      <c r="C90" s="582"/>
-      <c r="D90" s="592"/>
-      <c r="E90" s="582"/>
+      <c r="B90" s="591"/>
+      <c r="C90" s="581"/>
+      <c r="D90" s="591"/>
+      <c r="E90" s="581"/>
       <c r="Z90" s="526" t="s">
         <v>397</v>
       </c>
@@ -29357,10 +29349,10 @@
       <c r="A91" s="526" t="s">
         <v>396</v>
       </c>
-      <c r="B91" s="593"/>
-      <c r="C91" s="583"/>
-      <c r="D91" s="593"/>
-      <c r="E91" s="583"/>
+      <c r="B91" s="592"/>
+      <c r="C91" s="582"/>
+      <c r="D91" s="592"/>
+      <c r="E91" s="582"/>
       <c r="Z91" s="527" t="s">
         <v>398</v>
       </c>
@@ -29377,10 +29369,10 @@
       <c r="A92" s="526" t="s">
         <v>397</v>
       </c>
-      <c r="B92" s="593"/>
-      <c r="C92" s="583"/>
-      <c r="D92" s="593"/>
-      <c r="E92" s="583"/>
+      <c r="B92" s="592"/>
+      <c r="C92" s="582"/>
+      <c r="D92" s="592"/>
+      <c r="E92" s="582"/>
       <c r="Z92" s="526" t="s">
         <v>399</v>
       </c>
@@ -29397,10 +29389,10 @@
       <c r="A93" s="527" t="s">
         <v>398</v>
       </c>
-      <c r="B93" s="584"/>
-      <c r="C93" s="582"/>
-      <c r="D93" s="584"/>
-      <c r="E93" s="582"/>
+      <c r="B93" s="583"/>
+      <c r="C93" s="581"/>
+      <c r="D93" s="583"/>
+      <c r="E93" s="581"/>
       <c r="Z93" s="526" t="s">
         <v>400</v>
       </c>
@@ -29417,19 +29409,19 @@
       <c r="A94" s="526" t="s">
         <v>399</v>
       </c>
-      <c r="B94" s="593"/>
-      <c r="C94" s="583"/>
-      <c r="D94" s="593"/>
-      <c r="E94" s="583"/>
+      <c r="B94" s="592"/>
+      <c r="C94" s="582"/>
+      <c r="D94" s="592"/>
+      <c r="E94" s="582"/>
     </row>
     <row r="95" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A95" s="526" t="s">
         <v>400</v>
       </c>
-      <c r="B95" s="593"/>
-      <c r="C95" s="583"/>
-      <c r="D95" s="593"/>
-      <c r="E95" s="583"/>
+      <c r="B95" s="592"/>
+      <c r="C95" s="582"/>
+      <c r="D95" s="592"/>
+      <c r="E95" s="582"/>
     </row>
     <row r="96" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A96" s="528"/>
@@ -29444,25 +29436,25 @@
       </c>
     </row>
     <row r="101" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="B101" s="721" t="s">
+      <c r="B101" s="732" t="s">
         <v>350</v>
       </c>
-      <c r="C101" s="722"/>
-      <c r="D101" s="721" t="s">
+      <c r="C101" s="733"/>
+      <c r="D101" s="732" t="s">
         <v>359</v>
       </c>
-      <c r="E101" s="722"/>
+      <c r="E101" s="733"/>
     </row>
     <row r="102" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A102" s="324"/>
-      <c r="B102" s="723" t="s">
+      <c r="B102" s="734" t="s">
         <v>258</v>
       </c>
-      <c r="C102" s="687"/>
-      <c r="D102" s="723" t="s">
+      <c r="C102" s="686"/>
+      <c r="D102" s="734" t="s">
         <v>258</v>
       </c>
-      <c r="E102" s="687"/>
+      <c r="E102" s="686"/>
       <c r="Z102" t="s">
         <v>455</v>
       </c>
@@ -29505,9 +29497,9 @@
       <c r="A104" s="525" t="s">
         <v>259</v>
       </c>
-      <c r="B104" s="594"/>
+      <c r="B104" s="593"/>
       <c r="C104" s="554"/>
-      <c r="D104" s="594"/>
+      <c r="D104" s="593"/>
       <c r="E104" s="554"/>
       <c r="Z104" s="526" t="s">
         <v>394</v>
@@ -29525,9 +29517,9 @@
       <c r="A105" s="526" t="s">
         <v>394</v>
       </c>
-      <c r="B105" s="594"/>
+      <c r="B105" s="593"/>
       <c r="C105" s="474"/>
-      <c r="D105" s="594"/>
+      <c r="D105" s="593"/>
       <c r="E105" s="474"/>
       <c r="Z105" s="525" t="s">
         <v>395</v>
@@ -29545,9 +29537,9 @@
       <c r="A106" s="525" t="s">
         <v>395</v>
       </c>
-      <c r="B106" s="594"/>
+      <c r="B106" s="593"/>
       <c r="C106" s="554"/>
-      <c r="D106" s="594"/>
+      <c r="D106" s="593"/>
       <c r="E106" s="554"/>
       <c r="Z106" s="526" t="s">
         <v>396</v>
@@ -29565,9 +29557,9 @@
       <c r="A107" s="526" t="s">
         <v>396</v>
       </c>
-      <c r="B107" s="595"/>
+      <c r="B107" s="594"/>
       <c r="C107" s="482"/>
-      <c r="D107" s="595"/>
+      <c r="D107" s="594"/>
       <c r="E107" s="482"/>
       <c r="Z107" s="526" t="s">
         <v>397</v>
@@ -29585,9 +29577,9 @@
       <c r="A108" s="526" t="s">
         <v>397</v>
       </c>
-      <c r="B108" s="595"/>
+      <c r="B108" s="594"/>
       <c r="C108" s="482"/>
-      <c r="D108" s="595"/>
+      <c r="D108" s="594"/>
       <c r="E108" s="482"/>
       <c r="Z108" s="527" t="s">
         <v>398</v>
@@ -29605,9 +29597,9 @@
       <c r="A109" s="527" t="s">
         <v>398</v>
       </c>
-      <c r="B109" s="596"/>
+      <c r="B109" s="595"/>
       <c r="C109" s="554"/>
-      <c r="D109" s="596"/>
+      <c r="D109" s="595"/>
       <c r="E109" s="554"/>
       <c r="Z109" s="526" t="s">
         <v>399</v>
@@ -29625,9 +29617,9 @@
       <c r="A110" s="526" t="s">
         <v>399</v>
       </c>
-      <c r="B110" s="595"/>
+      <c r="B110" s="594"/>
       <c r="C110" s="482"/>
-      <c r="D110" s="595"/>
+      <c r="D110" s="594"/>
       <c r="E110" s="482"/>
       <c r="Z110" s="526" t="s">
         <v>400</v>
@@ -29645,9 +29637,9 @@
       <c r="A111" s="526" t="s">
         <v>400</v>
       </c>
-      <c r="B111" s="595"/>
+      <c r="B111" s="594"/>
       <c r="C111" s="482"/>
-      <c r="D111" s="595"/>
+      <c r="D111" s="594"/>
       <c r="E111" s="482"/>
     </row>
     <row r="112" spans="1:28" x14ac:dyDescent="0.25">
@@ -29663,25 +29655,25 @@
       </c>
     </row>
     <row r="116" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="B116" s="724" t="s">
+      <c r="B116" s="735" t="s">
         <v>350</v>
       </c>
-      <c r="C116" s="725"/>
-      <c r="D116" s="724" t="s">
+      <c r="C116" s="736"/>
+      <c r="D116" s="735" t="s">
         <v>359</v>
       </c>
-      <c r="E116" s="725"/>
+      <c r="E116" s="736"/>
     </row>
     <row r="117" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A117" s="530"/>
-      <c r="B117" s="726" t="s">
+      <c r="B117" s="737" t="s">
         <v>258</v>
       </c>
-      <c r="C117" s="727"/>
-      <c r="D117" s="726" t="s">
+      <c r="C117" s="738"/>
+      <c r="D117" s="737" t="s">
         <v>258</v>
       </c>
-      <c r="E117" s="727"/>
+      <c r="E117" s="738"/>
       <c r="Z117" t="s">
         <v>455</v>
       </c>
@@ -29716,7 +29708,7 @@
         <f t="shared" ref="AA118:AA125" si="17">E119</f>
         <v>0</v>
       </c>
-      <c r="AB118" s="559">
+      <c r="AB118" s="558">
         <f t="shared" ref="AB118:AB125" si="18">C119</f>
         <v>0</v>
       </c>
@@ -29725,9 +29717,9 @@
       <c r="A119" s="525" t="s">
         <v>259</v>
       </c>
-      <c r="B119" s="594"/>
+      <c r="B119" s="593"/>
       <c r="C119" s="554"/>
-      <c r="D119" s="594"/>
+      <c r="D119" s="593"/>
       <c r="E119" s="554"/>
       <c r="I119" s="555"/>
       <c r="Z119" s="526" t="s">
@@ -29737,7 +29729,7 @@
         <f t="shared" si="17"/>
         <v>0</v>
       </c>
-      <c r="AB119" s="559">
+      <c r="AB119" s="558">
         <f t="shared" si="18"/>
         <v>0</v>
       </c>
@@ -29746,9 +29738,9 @@
       <c r="A120" s="526" t="s">
         <v>394</v>
       </c>
-      <c r="B120" s="594"/>
+      <c r="B120" s="593"/>
       <c r="C120" s="474"/>
-      <c r="D120" s="594"/>
+      <c r="D120" s="593"/>
       <c r="E120" s="474"/>
       <c r="I120" s="555"/>
       <c r="Z120" s="525" t="s">
@@ -29758,7 +29750,7 @@
         <f t="shared" si="17"/>
         <v>0</v>
       </c>
-      <c r="AB120" s="559">
+      <c r="AB120" s="558">
         <f t="shared" si="18"/>
         <v>0</v>
       </c>
@@ -29767,9 +29759,9 @@
       <c r="A121" s="525" t="s">
         <v>395</v>
       </c>
-      <c r="B121" s="594"/>
+      <c r="B121" s="593"/>
       <c r="C121" s="554"/>
-      <c r="D121" s="594"/>
+      <c r="D121" s="593"/>
       <c r="E121" s="554"/>
       <c r="I121" s="555"/>
       <c r="Z121" s="526" t="s">
@@ -29779,7 +29771,7 @@
         <f t="shared" si="17"/>
         <v>0</v>
       </c>
-      <c r="AB121" s="559">
+      <c r="AB121" s="558">
         <f t="shared" si="18"/>
         <v>0</v>
       </c>
@@ -29788,9 +29780,9 @@
       <c r="A122" s="526" t="s">
         <v>396</v>
       </c>
-      <c r="B122" s="595"/>
+      <c r="B122" s="594"/>
       <c r="C122" s="482"/>
-      <c r="D122" s="595"/>
+      <c r="D122" s="594"/>
       <c r="E122" s="482"/>
       <c r="I122" s="555"/>
       <c r="Z122" s="526" t="s">
@@ -29800,7 +29792,7 @@
         <f t="shared" si="17"/>
         <v>0</v>
       </c>
-      <c r="AB122" s="559">
+      <c r="AB122" s="558">
         <f t="shared" si="18"/>
         <v>0</v>
       </c>
@@ -29809,9 +29801,9 @@
       <c r="A123" s="526" t="s">
         <v>397</v>
       </c>
-      <c r="B123" s="595"/>
+      <c r="B123" s="594"/>
       <c r="C123" s="482"/>
-      <c r="D123" s="595"/>
+      <c r="D123" s="594"/>
       <c r="E123" s="482"/>
       <c r="I123" s="555"/>
       <c r="Z123" s="527" t="s">
@@ -29821,7 +29813,7 @@
         <f t="shared" si="17"/>
         <v>0</v>
       </c>
-      <c r="AB123" s="559">
+      <c r="AB123" s="558">
         <f t="shared" si="18"/>
         <v>0</v>
       </c>
@@ -29830,9 +29822,9 @@
       <c r="A124" s="527" t="s">
         <v>398</v>
       </c>
-      <c r="B124" s="596"/>
+      <c r="B124" s="595"/>
       <c r="C124" s="554"/>
-      <c r="D124" s="596"/>
+      <c r="D124" s="595"/>
       <c r="E124" s="554"/>
       <c r="I124" s="555"/>
       <c r="Z124" s="526" t="s">
@@ -29842,7 +29834,7 @@
         <f t="shared" si="17"/>
         <v>0</v>
       </c>
-      <c r="AB124" s="559">
+      <c r="AB124" s="558">
         <f t="shared" si="18"/>
         <v>0</v>
       </c>
@@ -29851,9 +29843,9 @@
       <c r="A125" s="526" t="s">
         <v>399</v>
       </c>
-      <c r="B125" s="595"/>
+      <c r="B125" s="594"/>
       <c r="C125" s="482"/>
-      <c r="D125" s="595"/>
+      <c r="D125" s="594"/>
       <c r="E125" s="482"/>
       <c r="I125" s="555"/>
       <c r="Z125" s="526" t="s">
@@ -29863,7 +29855,7 @@
         <f t="shared" si="17"/>
         <v>0</v>
       </c>
-      <c r="AB125" s="559">
+      <c r="AB125" s="558">
         <f t="shared" si="18"/>
         <v>0</v>
       </c>
@@ -29872,9 +29864,9 @@
       <c r="A126" s="526" t="s">
         <v>400</v>
       </c>
-      <c r="B126" s="595"/>
+      <c r="B126" s="594"/>
       <c r="C126" s="482"/>
-      <c r="D126" s="595"/>
+      <c r="D126" s="594"/>
       <c r="E126" s="482"/>
     </row>
     <row r="127" spans="1:28" x14ac:dyDescent="0.25">
@@ -29888,11 +29880,11 @@
       <c r="A129" s="534" t="s">
         <v>353</v>
       </c>
-      <c r="B129" s="719" t="s">
+      <c r="B129" s="730" t="s">
         <v>350</v>
       </c>
-      <c r="C129" s="720"/>
-      <c r="D129" s="720"/>
+      <c r="C129" s="731"/>
+      <c r="D129" s="731"/>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" s="535"/>
@@ -29910,73 +29902,73 @@
       <c r="A131" s="538" t="s">
         <v>403</v>
       </c>
-      <c r="B131" s="585"/>
-      <c r="C131" s="582"/>
-      <c r="D131" s="584"/>
+      <c r="B131" s="584"/>
+      <c r="C131" s="581"/>
+      <c r="D131" s="583"/>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" s="474" t="s">
         <v>404</v>
       </c>
-      <c r="B132" s="585"/>
-      <c r="C132" s="565"/>
-      <c r="D132" s="585"/>
+      <c r="B132" s="584"/>
+      <c r="C132" s="564"/>
+      <c r="D132" s="584"/>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" s="474" t="s">
         <v>261</v>
       </c>
-      <c r="B133" s="585"/>
-      <c r="C133" s="565"/>
-      <c r="D133" s="585"/>
+      <c r="B133" s="584"/>
+      <c r="C133" s="564"/>
+      <c r="D133" s="584"/>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" s="474" t="s">
         <v>405</v>
       </c>
-      <c r="B134" s="585"/>
-      <c r="C134" s="565"/>
-      <c r="D134" s="585"/>
+      <c r="B134" s="584"/>
+      <c r="C134" s="564"/>
+      <c r="D134" s="584"/>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" s="474" t="s">
         <v>406</v>
       </c>
-      <c r="B135" s="585"/>
-      <c r="C135" s="565"/>
-      <c r="D135" s="585"/>
+      <c r="B135" s="584"/>
+      <c r="C135" s="564"/>
+      <c r="D135" s="584"/>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" s="474" t="s">
         <v>407</v>
       </c>
-      <c r="B136" s="585"/>
-      <c r="C136" s="565"/>
-      <c r="D136" s="585"/>
+      <c r="B136" s="584"/>
+      <c r="C136" s="564"/>
+      <c r="D136" s="584"/>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" s="474" t="s">
         <v>408</v>
       </c>
-      <c r="B137" s="585"/>
-      <c r="C137" s="565"/>
-      <c r="D137" s="585"/>
+      <c r="B137" s="584"/>
+      <c r="C137" s="564"/>
+      <c r="D137" s="584"/>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" s="474" t="s">
         <v>409</v>
       </c>
-      <c r="B138" s="585"/>
-      <c r="C138" s="565"/>
-      <c r="D138" s="585"/>
+      <c r="B138" s="584"/>
+      <c r="C138" s="564"/>
+      <c r="D138" s="584"/>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" s="474" t="s">
         <v>410</v>
       </c>
-      <c r="B139" s="585"/>
-      <c r="C139" s="565"/>
-      <c r="D139" s="585"/>
+      <c r="B139" s="584"/>
+      <c r="C139" s="564"/>
+      <c r="D139" s="584"/>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B140" s="539"/>
@@ -30183,7 +30175,7 @@
         <v>127</v>
       </c>
       <c r="C159" s="529"/>
-      <c r="D159" s="558"/>
+      <c r="D159" s="739"/>
       <c r="Z159" s="540" t="s">
         <v>411</v>
       </c>
@@ -30203,7 +30195,7 @@
         <v>127</v>
       </c>
       <c r="C160" s="529"/>
-      <c r="D160" s="558"/>
+      <c r="D160" s="739"/>
       <c r="Z160" s="544" t="s">
         <v>105</v>
       </c>
@@ -30227,7 +30219,7 @@
         <v>127</v>
       </c>
       <c r="C161" s="529"/>
-      <c r="D161" s="558"/>
+      <c r="D161" s="739"/>
       <c r="Z161" s="544" t="s">
         <v>110</v>
       </c>
@@ -30251,7 +30243,7 @@
         <v>127</v>
       </c>
       <c r="C162" s="529"/>
-      <c r="D162" s="558"/>
+      <c r="D162" s="739"/>
       <c r="Z162" s="544" t="s">
         <v>115</v>
       </c>
@@ -30539,13 +30531,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B22:C22"/>
     <mergeCell ref="B129:D129"/>
     <mergeCell ref="B85:C85"/>
     <mergeCell ref="D85:E85"/>
@@ -30559,6 +30544,13 @@
     <mergeCell ref="D116:E116"/>
     <mergeCell ref="B117:C117"/>
     <mergeCell ref="D117:E117"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B22:C22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="1200" r:id="rId1"/>
@@ -30814,123 +30806,123 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:95" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="630" t="s">
+      <c r="A1" s="600" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="631"/>
-      <c r="C1" s="631"/>
-      <c r="D1" s="631"/>
-      <c r="E1" s="631"/>
-      <c r="F1" s="631"/>
-      <c r="G1" s="631"/>
-      <c r="H1" s="632" t="s">
+      <c r="B1" s="601"/>
+      <c r="C1" s="601"/>
+      <c r="D1" s="601"/>
+      <c r="E1" s="601"/>
+      <c r="F1" s="601"/>
+      <c r="G1" s="601"/>
+      <c r="H1" s="602" t="s">
         <v>49</v>
       </c>
-      <c r="I1" s="633"/>
-      <c r="J1" s="633"/>
-      <c r="K1" s="633"/>
-      <c r="L1" s="633"/>
-      <c r="M1" s="634"/>
-      <c r="N1" s="635" t="s">
+      <c r="I1" s="603"/>
+      <c r="J1" s="603"/>
+      <c r="K1" s="603"/>
+      <c r="L1" s="603"/>
+      <c r="M1" s="604"/>
+      <c r="N1" s="605" t="s">
         <v>50</v>
       </c>
-      <c r="O1" s="613"/>
-      <c r="P1" s="613"/>
-      <c r="Q1" s="636"/>
-      <c r="R1" s="636"/>
-      <c r="S1" s="613"/>
-      <c r="T1" s="613"/>
-      <c r="U1" s="613"/>
-      <c r="V1" s="637" t="s">
+      <c r="O1" s="606"/>
+      <c r="P1" s="606"/>
+      <c r="Q1" s="607"/>
+      <c r="R1" s="607"/>
+      <c r="S1" s="606"/>
+      <c r="T1" s="606"/>
+      <c r="U1" s="606"/>
+      <c r="V1" s="608" t="s">
         <v>51</v>
       </c>
-      <c r="W1" s="638"/>
-      <c r="X1" s="639"/>
-      <c r="Y1" s="639"/>
-      <c r="Z1" s="640"/>
-      <c r="AA1" s="641" t="s">
+      <c r="W1" s="609"/>
+      <c r="X1" s="610"/>
+      <c r="Y1" s="610"/>
+      <c r="Z1" s="611"/>
+      <c r="AA1" s="612" t="s">
         <v>52</v>
       </c>
-      <c r="AB1" s="642"/>
-      <c r="AC1" s="642"/>
-      <c r="AD1" s="642"/>
-      <c r="AE1" s="642"/>
-      <c r="AF1" s="642"/>
-      <c r="AG1" s="642"/>
-      <c r="AH1" s="642"/>
-      <c r="AI1" s="642"/>
-      <c r="AJ1" s="642"/>
-      <c r="AK1" s="642"/>
-      <c r="AL1" s="642"/>
-      <c r="AM1" s="642"/>
+      <c r="AB1" s="613"/>
+      <c r="AC1" s="613"/>
+      <c r="AD1" s="613"/>
+      <c r="AE1" s="613"/>
+      <c r="AF1" s="613"/>
+      <c r="AG1" s="613"/>
+      <c r="AH1" s="613"/>
+      <c r="AI1" s="613"/>
+      <c r="AJ1" s="613"/>
+      <c r="AK1" s="613"/>
+      <c r="AL1" s="613"/>
+      <c r="AM1" s="613"/>
       <c r="AN1" s="7"/>
       <c r="AO1" s="8"/>
-      <c r="AP1" s="612" t="s">
+      <c r="AP1" s="625" t="s">
         <v>53</v>
       </c>
-      <c r="AQ1" s="613"/>
-      <c r="AR1" s="613"/>
-      <c r="AS1" s="613"/>
-      <c r="AT1" s="613"/>
-      <c r="AU1" s="613"/>
-      <c r="AV1" s="613"/>
-      <c r="AW1" s="614"/>
-      <c r="AX1" s="621" t="s">
+      <c r="AQ1" s="606"/>
+      <c r="AR1" s="606"/>
+      <c r="AS1" s="606"/>
+      <c r="AT1" s="606"/>
+      <c r="AU1" s="606"/>
+      <c r="AV1" s="606"/>
+      <c r="AW1" s="626"/>
+      <c r="AX1" s="633" t="s">
         <v>54</v>
       </c>
-      <c r="AY1" s="622"/>
-      <c r="AZ1" s="622"/>
-      <c r="BA1" s="622"/>
-      <c r="BB1" s="622"/>
-      <c r="BC1" s="623"/>
-      <c r="BD1" s="624" t="s">
+      <c r="AY1" s="634"/>
+      <c r="AZ1" s="634"/>
+      <c r="BA1" s="634"/>
+      <c r="BB1" s="634"/>
+      <c r="BC1" s="635"/>
+      <c r="BD1" s="636" t="s">
         <v>55</v>
       </c>
-      <c r="BE1" s="625"/>
-      <c r="BF1" s="625"/>
-      <c r="BG1" s="625"/>
-      <c r="BH1" s="625"/>
-      <c r="BI1" s="626"/>
-      <c r="BJ1" s="627" t="s">
+      <c r="BE1" s="637"/>
+      <c r="BF1" s="637"/>
+      <c r="BG1" s="637"/>
+      <c r="BH1" s="637"/>
+      <c r="BI1" s="638"/>
+      <c r="BJ1" s="639" t="s">
         <v>56</v>
       </c>
-      <c r="BK1" s="628"/>
-      <c r="BL1" s="628"/>
-      <c r="BM1" s="628"/>
-      <c r="BN1" s="628"/>
-      <c r="BO1" s="628"/>
-      <c r="BP1" s="629"/>
-      <c r="BQ1" s="601" t="s">
+      <c r="BK1" s="640"/>
+      <c r="BL1" s="640"/>
+      <c r="BM1" s="640"/>
+      <c r="BN1" s="640"/>
+      <c r="BO1" s="640"/>
+      <c r="BP1" s="641"/>
+      <c r="BQ1" s="614" t="s">
         <v>57</v>
       </c>
-      <c r="BR1" s="602"/>
-      <c r="BS1" s="602"/>
-      <c r="BT1" s="602"/>
-      <c r="BU1" s="602"/>
-      <c r="BV1" s="602"/>
+      <c r="BR1" s="615"/>
+      <c r="BS1" s="615"/>
+      <c r="BT1" s="615"/>
+      <c r="BU1" s="615"/>
+      <c r="BV1" s="615"/>
       <c r="BW1" s="8"/>
       <c r="BX1" s="9"/>
-      <c r="BY1" s="603" t="s">
+      <c r="BY1" s="616" t="s">
         <v>58</v>
       </c>
-      <c r="BZ1" s="604"/>
-      <c r="CA1" s="604"/>
-      <c r="CB1" s="604"/>
-      <c r="CC1" s="604"/>
-      <c r="CD1" s="604"/>
-      <c r="CE1" s="604"/>
-      <c r="CF1" s="605"/>
-      <c r="CG1" s="605"/>
-      <c r="CH1" s="605"/>
-      <c r="CI1" s="605"/>
-      <c r="CJ1" s="605"/>
-      <c r="CK1" s="605"/>
-      <c r="CL1" s="605"/>
-      <c r="CM1" s="605"/>
-      <c r="CN1" s="605"/>
-      <c r="CO1" s="605"/>
-      <c r="CP1" s="605"/>
-      <c r="CQ1" s="605"/>
+      <c r="BZ1" s="617"/>
+      <c r="CA1" s="617"/>
+      <c r="CB1" s="617"/>
+      <c r="CC1" s="617"/>
+      <c r="CD1" s="617"/>
+      <c r="CE1" s="617"/>
+      <c r="CF1" s="618"/>
+      <c r="CG1" s="618"/>
+      <c r="CH1" s="618"/>
+      <c r="CI1" s="618"/>
+      <c r="CJ1" s="618"/>
+      <c r="CK1" s="618"/>
+      <c r="CL1" s="618"/>
+      <c r="CM1" s="618"/>
+      <c r="CN1" s="618"/>
+      <c r="CO1" s="618"/>
+      <c r="CP1" s="618"/>
+      <c r="CQ1" s="618"/>
     </row>
     <row r="2" spans="1:95" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
@@ -30954,18 +30946,18 @@
       <c r="G2" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="H2" s="606" t="s">
+      <c r="H2" s="619" t="s">
         <v>66</v>
       </c>
-      <c r="I2" s="607"/>
-      <c r="J2" s="607" t="s">
+      <c r="I2" s="620"/>
+      <c r="J2" s="620" t="s">
         <v>67</v>
       </c>
-      <c r="K2" s="607"/>
-      <c r="L2" s="607" t="s">
+      <c r="K2" s="620"/>
+      <c r="L2" s="620" t="s">
         <v>68</v>
       </c>
-      <c r="M2" s="608"/>
+      <c r="M2" s="621"/>
       <c r="N2" s="12" t="s">
         <v>59</v>
       </c>
@@ -31074,36 +31066,36 @@
       <c r="AW2" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="AX2" s="609" t="s">
+      <c r="AX2" s="622" t="s">
         <v>93</v>
       </c>
-      <c r="AY2" s="610"/>
-      <c r="AZ2" s="610"/>
-      <c r="BA2" s="610" t="s">
+      <c r="AY2" s="623"/>
+      <c r="AZ2" s="623"/>
+      <c r="BA2" s="623" t="s">
         <v>94</v>
       </c>
-      <c r="BB2" s="610"/>
-      <c r="BC2" s="611"/>
-      <c r="BD2" s="615" t="s">
+      <c r="BB2" s="623"/>
+      <c r="BC2" s="624"/>
+      <c r="BD2" s="627" t="s">
         <v>93</v>
       </c>
-      <c r="BE2" s="616"/>
-      <c r="BF2" s="616"/>
-      <c r="BG2" s="616" t="s">
+      <c r="BE2" s="628"/>
+      <c r="BF2" s="628"/>
+      <c r="BG2" s="628" t="s">
         <v>94</v>
       </c>
-      <c r="BH2" s="616"/>
-      <c r="BI2" s="617"/>
-      <c r="BJ2" s="618" t="s">
+      <c r="BH2" s="628"/>
+      <c r="BI2" s="629"/>
+      <c r="BJ2" s="630" t="s">
         <v>93</v>
       </c>
-      <c r="BK2" s="619"/>
-      <c r="BL2" s="619"/>
-      <c r="BM2" s="619" t="s">
+      <c r="BK2" s="631"/>
+      <c r="BL2" s="631"/>
+      <c r="BM2" s="631" t="s">
         <v>94</v>
       </c>
-      <c r="BN2" s="620"/>
-      <c r="BO2" s="620"/>
+      <c r="BN2" s="632"/>
+      <c r="BO2" s="632"/>
       <c r="BP2" s="24" t="s">
         <v>95</v>
       </c>
@@ -31976,11 +31968,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="H1:M1"/>
-    <mergeCell ref="N1:U1"/>
-    <mergeCell ref="V1:Z1"/>
-    <mergeCell ref="AA1:AM1"/>
     <mergeCell ref="BQ1:BV1"/>
     <mergeCell ref="BY1:CQ1"/>
     <mergeCell ref="H2:I2"/>
@@ -31996,6 +31983,11 @@
     <mergeCell ref="AX1:BC1"/>
     <mergeCell ref="BD1:BI1"/>
     <mergeCell ref="BJ1:BP1"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="H1:M1"/>
+    <mergeCell ref="N1:U1"/>
+    <mergeCell ref="V1:Z1"/>
+    <mergeCell ref="AA1:AM1"/>
   </mergeCells>
   <conditionalFormatting sqref="A13:A14 A4:B4">
     <cfRule type="duplicateValues" dxfId="8" priority="1"/>
@@ -32032,124 +32024,124 @@
         <v>138</v>
       </c>
       <c r="L1" s="93"/>
-      <c r="M1" s="669" t="s">
+      <c r="M1" s="646" t="s">
         <v>139</v>
       </c>
-      <c r="N1" s="670" t="s">
+      <c r="N1" s="647" t="s">
         <v>140</v>
       </c>
-      <c r="O1" s="671"/>
-      <c r="P1" s="671"/>
-      <c r="Q1" s="671"/>
-      <c r="R1" s="672" t="s">
+      <c r="O1" s="648"/>
+      <c r="P1" s="648"/>
+      <c r="Q1" s="648"/>
+      <c r="R1" s="649" t="s">
         <v>141</v>
       </c>
-      <c r="S1" s="664"/>
-      <c r="T1" s="664"/>
-      <c r="U1" s="664"/>
-      <c r="V1" s="664"/>
-      <c r="W1" s="664"/>
-      <c r="X1" s="673"/>
-      <c r="Y1" s="653" t="s">
+      <c r="S1" s="650"/>
+      <c r="T1" s="650"/>
+      <c r="U1" s="650"/>
+      <c r="V1" s="650"/>
+      <c r="W1" s="650"/>
+      <c r="X1" s="651"/>
+      <c r="Y1" s="652" t="s">
         <v>142</v>
       </c>
-      <c r="Z1" s="625"/>
-      <c r="AA1" s="674" t="s">
+      <c r="Z1" s="637"/>
+      <c r="AA1" s="655" t="s">
         <v>143</v>
       </c>
-      <c r="AB1" s="665" t="s">
+      <c r="AB1" s="657" t="s">
         <v>144</v>
       </c>
-      <c r="AC1" s="660" t="s">
+      <c r="AC1" s="665" t="s">
         <v>145</v>
       </c>
-      <c r="AD1" s="661"/>
-      <c r="AE1" s="661"/>
-      <c r="AF1" s="662"/>
-      <c r="AG1" s="663" t="s">
+      <c r="AD1" s="666"/>
+      <c r="AE1" s="666"/>
+      <c r="AF1" s="667"/>
+      <c r="AG1" s="668" t="s">
         <v>146</v>
       </c>
-      <c r="AH1" s="664"/>
-      <c r="AI1" s="664"/>
-      <c r="AJ1" s="664"/>
-      <c r="AK1" s="664"/>
-      <c r="AL1" s="664"/>
-      <c r="AM1" s="664"/>
-      <c r="AN1" s="664"/>
-      <c r="AO1" s="665" t="s">
+      <c r="AH1" s="650"/>
+      <c r="AI1" s="650"/>
+      <c r="AJ1" s="650"/>
+      <c r="AK1" s="650"/>
+      <c r="AL1" s="650"/>
+      <c r="AM1" s="650"/>
+      <c r="AN1" s="650"/>
+      <c r="AO1" s="657" t="s">
         <v>147</v>
       </c>
-      <c r="AP1" s="653" t="s">
+      <c r="AP1" s="652" t="s">
         <v>148</v>
       </c>
-      <c r="AQ1" s="625"/>
-      <c r="AR1" s="625"/>
-      <c r="AS1" s="626"/>
-      <c r="AT1" s="667" t="s">
+      <c r="AQ1" s="637"/>
+      <c r="AR1" s="637"/>
+      <c r="AS1" s="638"/>
+      <c r="AT1" s="669" t="s">
         <v>149</v>
       </c>
-      <c r="AU1" s="668"/>
-      <c r="AV1" s="668"/>
-      <c r="AW1" s="668"/>
-      <c r="AX1" s="668"/>
-      <c r="AY1" s="668"/>
-      <c r="AZ1" s="668"/>
-      <c r="BA1" s="668"/>
-      <c r="BB1" s="668"/>
-      <c r="BC1" s="668"/>
-      <c r="BD1" s="668"/>
-      <c r="BE1" s="668"/>
-      <c r="BF1" s="668"/>
-      <c r="BG1" s="668"/>
-      <c r="BH1" s="668"/>
-      <c r="BI1" s="668"/>
-      <c r="BJ1" s="668"/>
-      <c r="BK1" s="668"/>
-      <c r="BL1" s="668"/>
-      <c r="BM1" s="668"/>
-      <c r="BN1" s="668"/>
-      <c r="BO1" s="668"/>
-      <c r="BP1" s="668"/>
-      <c r="BQ1" s="668"/>
-      <c r="BR1" s="668"/>
-      <c r="BS1" s="668"/>
-      <c r="BT1" s="668"/>
-      <c r="BU1" s="668"/>
-      <c r="BV1" s="668"/>
-      <c r="BW1" s="665" t="s">
+      <c r="AU1" s="670"/>
+      <c r="AV1" s="670"/>
+      <c r="AW1" s="670"/>
+      <c r="AX1" s="670"/>
+      <c r="AY1" s="670"/>
+      <c r="AZ1" s="670"/>
+      <c r="BA1" s="670"/>
+      <c r="BB1" s="670"/>
+      <c r="BC1" s="670"/>
+      <c r="BD1" s="670"/>
+      <c r="BE1" s="670"/>
+      <c r="BF1" s="670"/>
+      <c r="BG1" s="670"/>
+      <c r="BH1" s="670"/>
+      <c r="BI1" s="670"/>
+      <c r="BJ1" s="670"/>
+      <c r="BK1" s="670"/>
+      <c r="BL1" s="670"/>
+      <c r="BM1" s="670"/>
+      <c r="BN1" s="670"/>
+      <c r="BO1" s="670"/>
+      <c r="BP1" s="670"/>
+      <c r="BQ1" s="670"/>
+      <c r="BR1" s="670"/>
+      <c r="BS1" s="670"/>
+      <c r="BT1" s="670"/>
+      <c r="BU1" s="670"/>
+      <c r="BV1" s="670"/>
+      <c r="BW1" s="657" t="s">
         <v>150</v>
       </c>
-      <c r="BX1" s="653" t="s">
+      <c r="BX1" s="652" t="s">
         <v>151</v>
       </c>
-      <c r="BY1" s="625"/>
-      <c r="BZ1" s="625"/>
-      <c r="CA1" s="626"/>
-      <c r="CB1" s="654" t="s">
+      <c r="BY1" s="637"/>
+      <c r="BZ1" s="637"/>
+      <c r="CA1" s="638"/>
+      <c r="CB1" s="659" t="s">
         <v>52</v>
       </c>
-      <c r="CC1" s="654"/>
-      <c r="CD1" s="654"/>
-      <c r="CE1" s="654"/>
-      <c r="CF1" s="654"/>
-      <c r="CG1" s="654"/>
-      <c r="CH1" s="654"/>
-      <c r="CI1" s="654"/>
-      <c r="CJ1" s="654"/>
-      <c r="CK1" s="654"/>
-      <c r="CL1" s="654"/>
-      <c r="CM1" s="654"/>
+      <c r="CC1" s="659"/>
+      <c r="CD1" s="659"/>
+      <c r="CE1" s="659"/>
+      <c r="CF1" s="659"/>
+      <c r="CG1" s="659"/>
+      <c r="CH1" s="659"/>
+      <c r="CI1" s="659"/>
+      <c r="CJ1" s="659"/>
+      <c r="CK1" s="659"/>
+      <c r="CL1" s="659"/>
+      <c r="CM1" s="659"/>
       <c r="CN1" s="94"/>
-      <c r="CO1" s="655" t="s">
+      <c r="CO1" s="660" t="s">
         <v>57</v>
       </c>
-      <c r="CP1" s="613"/>
-      <c r="CQ1" s="613"/>
-      <c r="CR1" s="613"/>
-      <c r="CS1" s="613"/>
-      <c r="CT1" s="613"/>
-      <c r="CU1" s="613"/>
-      <c r="CV1" s="614"/>
+      <c r="CP1" s="606"/>
+      <c r="CQ1" s="606"/>
+      <c r="CR1" s="606"/>
+      <c r="CS1" s="606"/>
+      <c r="CT1" s="606"/>
+      <c r="CU1" s="606"/>
+      <c r="CV1" s="626"/>
     </row>
     <row r="2" spans="1:100" ht="64.5" x14ac:dyDescent="0.25">
       <c r="A2" s="95" t="s">
@@ -32188,7 +32180,7 @@
       <c r="L2" s="99" t="s">
         <v>60</v>
       </c>
-      <c r="M2" s="669"/>
+      <c r="M2" s="646"/>
       <c r="N2" s="100" t="s">
         <v>156</v>
       </c>
@@ -32204,22 +32196,22 @@
       <c r="R2" s="101" t="s">
         <v>439</v>
       </c>
-      <c r="S2" s="656" t="s">
+      <c r="S2" s="661" t="s">
         <v>159</v>
       </c>
-      <c r="T2" s="620"/>
-      <c r="U2" s="657" t="s">
+      <c r="T2" s="632"/>
+      <c r="U2" s="662" t="s">
         <v>67</v>
       </c>
-      <c r="V2" s="657"/>
-      <c r="W2" s="657" t="s">
+      <c r="V2" s="662"/>
+      <c r="W2" s="662" t="s">
         <v>68</v>
       </c>
-      <c r="X2" s="658"/>
-      <c r="Y2" s="647"/>
-      <c r="Z2" s="648"/>
-      <c r="AA2" s="675"/>
-      <c r="AB2" s="666"/>
+      <c r="X2" s="663"/>
+      <c r="Y2" s="653"/>
+      <c r="Z2" s="654"/>
+      <c r="AA2" s="656"/>
+      <c r="AB2" s="658"/>
       <c r="AC2" s="102" t="s">
         <v>160</v>
       </c>
@@ -32232,81 +32224,81 @@
       <c r="AF2" s="102" t="s">
         <v>163</v>
       </c>
-      <c r="AG2" s="659" t="s">
+      <c r="AG2" s="664" t="s">
         <v>164</v>
       </c>
-      <c r="AH2" s="645"/>
-      <c r="AI2" s="645" t="s">
+      <c r="AH2" s="644"/>
+      <c r="AI2" s="644" t="s">
         <v>165</v>
       </c>
-      <c r="AJ2" s="645"/>
-      <c r="AK2" s="645" t="s">
+      <c r="AJ2" s="644"/>
+      <c r="AK2" s="644" t="s">
         <v>166</v>
       </c>
-      <c r="AL2" s="645"/>
+      <c r="AL2" s="644"/>
       <c r="AM2" s="103" t="s">
         <v>167</v>
       </c>
       <c r="AN2" s="103" t="s">
         <v>168</v>
       </c>
-      <c r="AO2" s="666"/>
-      <c r="AP2" s="647" t="s">
+      <c r="AO2" s="658"/>
+      <c r="AP2" s="653" t="s">
         <v>169</v>
       </c>
-      <c r="AQ2" s="648"/>
-      <c r="AR2" s="649" t="s">
+      <c r="AQ2" s="654"/>
+      <c r="AR2" s="642" t="s">
         <v>170</v>
       </c>
-      <c r="AS2" s="650"/>
-      <c r="AT2" s="645" t="s">
+      <c r="AS2" s="643"/>
+      <c r="AT2" s="644" t="s">
         <v>171</v>
       </c>
-      <c r="AU2" s="645"/>
-      <c r="AV2" s="646" t="s">
+      <c r="AU2" s="644"/>
+      <c r="AV2" s="645" t="s">
         <v>172</v>
       </c>
-      <c r="AW2" s="646"/>
-      <c r="AX2" s="646" t="s">
+      <c r="AW2" s="645"/>
+      <c r="AX2" s="645" t="s">
         <v>173</v>
       </c>
-      <c r="AY2" s="646"/>
+      <c r="AY2" s="645"/>
       <c r="AZ2" s="103" t="s">
         <v>174</v>
       </c>
       <c r="BA2" s="103" t="s">
         <v>175</v>
       </c>
-      <c r="BB2" s="645" t="s">
+      <c r="BB2" s="644" t="s">
         <v>176</v>
       </c>
-      <c r="BC2" s="645"/>
-      <c r="BD2" s="646" t="s">
+      <c r="BC2" s="644"/>
+      <c r="BD2" s="645" t="s">
         <v>177</v>
       </c>
-      <c r="BE2" s="646"/>
-      <c r="BF2" s="646" t="s">
+      <c r="BE2" s="645"/>
+      <c r="BF2" s="645" t="s">
         <v>178</v>
       </c>
-      <c r="BG2" s="646"/>
+      <c r="BG2" s="645"/>
       <c r="BH2" s="103" t="s">
         <v>179</v>
       </c>
       <c r="BI2" s="103" t="s">
         <v>180</v>
       </c>
-      <c r="BJ2" s="645" t="s">
+      <c r="BJ2" s="644" t="s">
         <v>181</v>
       </c>
-      <c r="BK2" s="645"/>
-      <c r="BL2" s="646" t="s">
+      <c r="BK2" s="644"/>
+      <c r="BL2" s="645" t="s">
         <v>182</v>
       </c>
-      <c r="BM2" s="646"/>
-      <c r="BN2" s="646" t="s">
+      <c r="BM2" s="645"/>
+      <c r="BN2" s="645" t="s">
         <v>183</v>
       </c>
-      <c r="BO2" s="646"/>
+      <c r="BO2" s="645"/>
       <c r="BP2" s="103" t="s">
         <v>184</v>
       </c>
@@ -32328,15 +32320,15 @@
       <c r="BV2" s="103" t="s">
         <v>190</v>
       </c>
-      <c r="BW2" s="666"/>
-      <c r="BX2" s="647" t="s">
+      <c r="BW2" s="658"/>
+      <c r="BX2" s="653" t="s">
         <v>169</v>
       </c>
-      <c r="BY2" s="648"/>
-      <c r="BZ2" s="649" t="s">
+      <c r="BY2" s="654"/>
+      <c r="BZ2" s="642" t="s">
         <v>170</v>
       </c>
-      <c r="CA2" s="650"/>
+      <c r="CA2" s="643"/>
       <c r="CB2" s="20" t="s">
         <v>74</v>
       </c>
@@ -32376,22 +32368,22 @@
       <c r="CN2" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="CO2" s="651" t="s">
+      <c r="CO2" s="673" t="s">
         <v>191</v>
       </c>
-      <c r="CP2" s="652"/>
-      <c r="CQ2" s="643" t="s">
+      <c r="CP2" s="674"/>
+      <c r="CQ2" s="671" t="s">
         <v>192</v>
       </c>
-      <c r="CR2" s="643"/>
-      <c r="CS2" s="652" t="s">
+      <c r="CR2" s="671"/>
+      <c r="CS2" s="674" t="s">
         <v>193</v>
       </c>
-      <c r="CT2" s="652"/>
-      <c r="CU2" s="643" t="s">
+      <c r="CT2" s="674"/>
+      <c r="CU2" s="671" t="s">
         <v>194</v>
       </c>
-      <c r="CV2" s="644"/>
+      <c r="CV2" s="672"/>
     </row>
     <row r="3" spans="1:100" ht="27" x14ac:dyDescent="0.25">
       <c r="A3" s="105" t="s">
@@ -37697,16 +37689,18 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="AR2:AS2"/>
-    <mergeCell ref="AT2:AU2"/>
-    <mergeCell ref="AV2:AW2"/>
-    <mergeCell ref="AX2:AY2"/>
-    <mergeCell ref="M1:M2"/>
-    <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="R1:X1"/>
-    <mergeCell ref="Y1:Z2"/>
-    <mergeCell ref="AA1:AA2"/>
-    <mergeCell ref="AB1:AB2"/>
+    <mergeCell ref="CU2:CV2"/>
+    <mergeCell ref="BB2:BC2"/>
+    <mergeCell ref="BD2:BE2"/>
+    <mergeCell ref="BF2:BG2"/>
+    <mergeCell ref="BJ2:BK2"/>
+    <mergeCell ref="BL2:BM2"/>
+    <mergeCell ref="BN2:BO2"/>
+    <mergeCell ref="BX2:BY2"/>
+    <mergeCell ref="BZ2:CA2"/>
+    <mergeCell ref="CO2:CP2"/>
+    <mergeCell ref="CQ2:CR2"/>
+    <mergeCell ref="CS2:CT2"/>
     <mergeCell ref="BX1:CA1"/>
     <mergeCell ref="CB1:CM1"/>
     <mergeCell ref="CO1:CV1"/>
@@ -37723,18 +37717,16 @@
     <mergeCell ref="AP1:AS1"/>
     <mergeCell ref="AT1:BV1"/>
     <mergeCell ref="BW1:BW2"/>
-    <mergeCell ref="CU2:CV2"/>
-    <mergeCell ref="BB2:BC2"/>
-    <mergeCell ref="BD2:BE2"/>
-    <mergeCell ref="BF2:BG2"/>
-    <mergeCell ref="BJ2:BK2"/>
-    <mergeCell ref="BL2:BM2"/>
-    <mergeCell ref="BN2:BO2"/>
-    <mergeCell ref="BX2:BY2"/>
-    <mergeCell ref="BZ2:CA2"/>
-    <mergeCell ref="CO2:CP2"/>
-    <mergeCell ref="CQ2:CR2"/>
-    <mergeCell ref="CS2:CT2"/>
+    <mergeCell ref="AR2:AS2"/>
+    <mergeCell ref="AT2:AU2"/>
+    <mergeCell ref="AV2:AW2"/>
+    <mergeCell ref="AX2:AY2"/>
+    <mergeCell ref="M1:M2"/>
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="R1:X1"/>
+    <mergeCell ref="Y1:Z2"/>
+    <mergeCell ref="AA1:AA2"/>
+    <mergeCell ref="AB1:AB2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -37787,8 +37779,8 @@
       <c r="B2" s="218" t="s">
         <v>213</v>
       </c>
-      <c r="C2" s="683"/>
-      <c r="D2" s="683"/>
+      <c r="C2" s="675"/>
+      <c r="D2" s="675"/>
       <c r="E2" s="216"/>
       <c r="F2" s="216"/>
       <c r="G2" s="216"/>
@@ -37913,32 +37905,32 @@
     </row>
     <row r="7" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="215"/>
-      <c r="B7" s="684" t="s">
+      <c r="B7" s="676" t="s">
         <v>217</v>
       </c>
-      <c r="C7" s="684"/>
-      <c r="D7" s="684"/>
+      <c r="C7" s="676"/>
+      <c r="D7" s="676"/>
       <c r="E7" s="216"/>
       <c r="F7" s="216"/>
       <c r="G7" s="216"/>
       <c r="H7" s="216"/>
       <c r="I7" s="216"/>
-      <c r="J7" s="684" t="s">
+      <c r="J7" s="676" t="s">
         <v>218</v>
       </c>
-      <c r="K7" s="684"/>
-      <c r="L7" s="684"/>
+      <c r="K7" s="676"/>
+      <c r="L7" s="676"/>
       <c r="M7" s="216"/>
       <c r="N7" s="216"/>
       <c r="O7" s="216"/>
       <c r="P7" s="217" t="s">
         <v>219</v>
       </c>
-      <c r="Q7" s="684" t="s">
+      <c r="Q7" s="676" t="s">
         <v>218</v>
       </c>
-      <c r="R7" s="684"/>
-      <c r="S7" s="684"/>
+      <c r="R7" s="676"/>
+      <c r="S7" s="676"/>
       <c r="T7" s="216"/>
       <c r="U7" s="230" t="s">
         <v>220</v>
@@ -37972,41 +37964,41 @@
       <c r="B9" s="231" t="s">
         <v>221</v>
       </c>
-      <c r="C9" s="679" t="s">
+      <c r="C9" s="677" t="s">
         <v>222</v>
       </c>
-      <c r="D9" s="680"/>
-      <c r="E9" s="679" t="s">
+      <c r="D9" s="678"/>
+      <c r="E9" s="677" t="s">
         <v>223</v>
       </c>
-      <c r="F9" s="680"/>
+      <c r="F9" s="678"/>
       <c r="G9" s="216"/>
       <c r="H9" s="216"/>
       <c r="I9" s="216"/>
       <c r="J9" s="231" t="s">
         <v>221</v>
       </c>
-      <c r="K9" s="679" t="s">
+      <c r="K9" s="677" t="s">
         <v>222</v>
       </c>
-      <c r="L9" s="680"/>
-      <c r="M9" s="679" t="s">
+      <c r="L9" s="678"/>
+      <c r="M9" s="677" t="s">
         <v>223</v>
       </c>
-      <c r="N9" s="680"/>
+      <c r="N9" s="678"/>
       <c r="O9" s="216"/>
       <c r="P9" s="216"/>
       <c r="Q9" s="231" t="s">
         <v>221</v>
       </c>
-      <c r="R9" s="679" t="s">
+      <c r="R9" s="677" t="s">
         <v>222</v>
       </c>
-      <c r="S9" s="680"/>
-      <c r="T9" s="679" t="s">
+      <c r="S9" s="678"/>
+      <c r="T9" s="677" t="s">
         <v>223</v>
       </c>
-      <c r="U9" s="680"/>
+      <c r="U9" s="678"/>
     </row>
     <row r="10" spans="1:21" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="215"/>
@@ -38068,10 +38060,10 @@
       </c>
       <c r="C11" s="236"/>
       <c r="D11" s="236"/>
-      <c r="E11" s="676" t="s">
+      <c r="E11" s="679" t="s">
         <v>228</v>
       </c>
-      <c r="F11" s="677"/>
+      <c r="F11" s="680"/>
       <c r="G11" s="237"/>
       <c r="H11" s="237"/>
       <c r="I11" s="237"/>
@@ -38080,10 +38072,10 @@
       </c>
       <c r="K11" s="216"/>
       <c r="L11" s="216"/>
-      <c r="M11" s="681" t="s">
+      <c r="M11" s="682" t="s">
         <v>228</v>
       </c>
-      <c r="N11" s="682"/>
+      <c r="N11" s="683"/>
       <c r="O11" s="237"/>
       <c r="P11" s="237"/>
       <c r="Q11" s="235" t="s">
@@ -38091,10 +38083,10 @@
       </c>
       <c r="R11" s="236"/>
       <c r="S11" s="236"/>
-      <c r="T11" s="676" t="s">
+      <c r="T11" s="679" t="s">
         <v>228</v>
       </c>
-      <c r="U11" s="677"/>
+      <c r="U11" s="680"/>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="215"/>
@@ -38337,10 +38329,10 @@
       </c>
       <c r="C20" s="274"/>
       <c r="D20" s="274"/>
-      <c r="E20" s="676" t="s">
+      <c r="E20" s="679" t="s">
         <v>237</v>
       </c>
-      <c r="F20" s="677"/>
+      <c r="F20" s="680"/>
       <c r="G20" s="251"/>
       <c r="H20" s="251"/>
       <c r="I20" s="216"/>
@@ -38349,10 +38341,10 @@
       </c>
       <c r="K20" s="274"/>
       <c r="L20" s="274"/>
-      <c r="M20" s="676" t="s">
+      <c r="M20" s="679" t="s">
         <v>237</v>
       </c>
-      <c r="N20" s="677"/>
+      <c r="N20" s="680"/>
       <c r="O20" s="264"/>
       <c r="P20" s="264"/>
       <c r="Q20" s="235" t="s">
@@ -38360,10 +38352,10 @@
       </c>
       <c r="R20" s="274"/>
       <c r="S20" s="274"/>
-      <c r="T20" s="676" t="s">
+      <c r="T20" s="679" t="s">
         <v>237</v>
       </c>
-      <c r="U20" s="677"/>
+      <c r="U20" s="680"/>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" s="215"/>
@@ -38452,7 +38444,7 @@
       <c r="T23" s="262"/>
       <c r="U23" s="263"/>
     </row>
-    <row r="24" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:21" ht="24" x14ac:dyDescent="0.25">
       <c r="A24" s="215"/>
       <c r="B24" s="280" t="s">
         <v>239</v>
@@ -38659,10 +38651,10 @@
       </c>
       <c r="C30" s="274"/>
       <c r="D30" s="274"/>
-      <c r="E30" s="676" t="s">
+      <c r="E30" s="679" t="s">
         <v>237</v>
       </c>
-      <c r="F30" s="677"/>
+      <c r="F30" s="680"/>
       <c r="G30" s="251"/>
       <c r="H30" s="251"/>
       <c r="I30" s="216"/>
@@ -38671,10 +38663,10 @@
       </c>
       <c r="K30" s="274"/>
       <c r="L30" s="274"/>
-      <c r="M30" s="676" t="s">
+      <c r="M30" s="679" t="s">
         <v>237</v>
       </c>
-      <c r="N30" s="677"/>
+      <c r="N30" s="680"/>
       <c r="O30" s="264"/>
       <c r="P30" s="264"/>
       <c r="Q30" s="235" t="s">
@@ -38682,10 +38674,10 @@
       </c>
       <c r="R30" s="274"/>
       <c r="S30" s="274"/>
-      <c r="T30" s="676" t="s">
+      <c r="T30" s="679" t="s">
         <v>237</v>
       </c>
-      <c r="U30" s="677"/>
+      <c r="U30" s="680"/>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A31" s="290"/>
@@ -39064,11 +39056,11 @@
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A42" s="215"/>
-      <c r="B42" s="678"/>
-      <c r="C42" s="678"/>
-      <c r="D42" s="678"/>
-      <c r="E42" s="678"/>
-      <c r="F42" s="678"/>
+      <c r="B42" s="681"/>
+      <c r="C42" s="681"/>
+      <c r="D42" s="681"/>
+      <c r="E42" s="681"/>
+      <c r="F42" s="681"/>
       <c r="G42" s="264"/>
       <c r="H42" s="216"/>
       <c r="I42" s="264"/>
@@ -39212,15 +39204,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="J7:L7"/>
-    <mergeCell ref="Q7:S7"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="M9:N9"/>
-    <mergeCell ref="R9:S9"/>
     <mergeCell ref="E30:F30"/>
     <mergeCell ref="M30:N30"/>
     <mergeCell ref="T30:U30"/>
@@ -39232,6 +39215,15 @@
     <mergeCell ref="E20:F20"/>
     <mergeCell ref="M20:N20"/>
     <mergeCell ref="T20:U20"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="Q7:S7"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="R9:S9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -39261,8 +39253,8 @@
       <c r="B3" s="317" t="s">
         <v>213</v>
       </c>
-      <c r="C3" s="685"/>
-      <c r="D3" s="685"/>
+      <c r="C3" s="684"/>
+      <c r="D3" s="684"/>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C4" s="318"/>
@@ -39295,10 +39287,10 @@
       <c r="D10" s="326" t="s">
         <v>257</v>
       </c>
-      <c r="E10" s="686" t="s">
+      <c r="E10" s="685" t="s">
         <v>258</v>
       </c>
-      <c r="F10" s="687"/>
+      <c r="F10" s="686"/>
     </row>
     <row r="11" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="327" t="s">
@@ -39447,10 +39439,10 @@
       <c r="D30" s="339" t="s">
         <v>257</v>
       </c>
-      <c r="E30" s="686" t="s">
+      <c r="E30" s="685" t="s">
         <v>258</v>
       </c>
-      <c r="F30" s="687"/>
+      <c r="F30" s="686"/>
     </row>
     <row r="31" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="327" t="s">
@@ -39596,10 +39588,10 @@
       <c r="D49" s="339" t="s">
         <v>257</v>
       </c>
-      <c r="E49" s="686" t="s">
+      <c r="E49" s="685" t="s">
         <v>258</v>
       </c>
-      <c r="F49" s="687"/>
+      <c r="F49" s="686"/>
     </row>
     <row r="50" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B50" s="327" t="s">
@@ -39763,8 +39755,8 @@
       </c>
       <c r="C2" s="218"/>
       <c r="D2" s="218"/>
-      <c r="E2" s="683"/>
-      <c r="F2" s="683"/>
+      <c r="E2" s="675"/>
+      <c r="F2" s="675"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="217"/>
@@ -39796,13 +39788,13 @@
     </row>
     <row r="6" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="215"/>
-      <c r="B6" s="684" t="s">
+      <c r="B6" s="676" t="s">
         <v>270</v>
       </c>
-      <c r="C6" s="684"/>
-      <c r="D6" s="684"/>
-      <c r="E6" s="684"/>
-      <c r="F6" s="684"/>
+      <c r="C6" s="676"/>
+      <c r="D6" s="676"/>
+      <c r="E6" s="676"/>
+      <c r="F6" s="676"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="215"/>
@@ -39817,14 +39809,14 @@
       <c r="B8" s="342" t="s">
         <v>221</v>
       </c>
-      <c r="C8" s="688" t="s">
+      <c r="C8" s="687" t="s">
         <v>222</v>
       </c>
-      <c r="D8" s="688"/>
-      <c r="E8" s="688" t="s">
+      <c r="D8" s="687"/>
+      <c r="E8" s="687" t="s">
         <v>223</v>
       </c>
-      <c r="F8" s="689"/>
+      <c r="F8" s="688"/>
     </row>
     <row r="9" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="215"/>
@@ -39879,8 +39871,8 @@
       <c r="B13" s="253"/>
       <c r="C13" s="358"/>
       <c r="D13" s="358"/>
-      <c r="E13" s="690"/>
-      <c r="F13" s="691"/>
+      <c r="E13" s="689"/>
+      <c r="F13" s="690"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="346"/>
@@ -39960,11 +39952,11 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="215"/>
-      <c r="B22" s="678"/>
-      <c r="C22" s="678"/>
-      <c r="D22" s="678"/>
-      <c r="E22" s="678"/>
-      <c r="F22" s="678"/>
+      <c r="B22" s="681"/>
+      <c r="C22" s="681"/>
+      <c r="D22" s="681"/>
+      <c r="E22" s="681"/>
+      <c r="F22" s="681"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="215"/>
@@ -40028,13 +40020,13 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="1:14" ht="51" x14ac:dyDescent="0.25">
-      <c r="B2" s="692" t="s">
+      <c r="B2" s="691" t="s">
         <v>277</v>
       </c>
-      <c r="C2" s="693" t="s">
+      <c r="C2" s="692" t="s">
         <v>278</v>
       </c>
-      <c r="D2" s="693" t="s">
+      <c r="D2" s="692" t="s">
         <v>154</v>
       </c>
       <c r="E2" s="372" t="s">
@@ -40069,9 +40061,9 @@
       </c>
     </row>
     <row r="3" spans="1:14" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B3" s="692"/>
-      <c r="C3" s="694"/>
-      <c r="D3" s="694"/>
+      <c r="B3" s="691"/>
+      <c r="C3" s="693"/>
+      <c r="D3" s="693"/>
       <c r="E3" s="374" t="s">
         <v>287</v>
       </c>
@@ -40104,7 +40096,7 @@
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B4" s="695" t="s">
+      <c r="B4" s="694" t="s">
         <v>290</v>
       </c>
       <c r="C4" s="376" t="s">
@@ -40123,7 +40115,7 @@
       <c r="N4" s="378"/>
     </row>
     <row r="5" spans="1:14" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B5" s="695"/>
+      <c r="B5" s="694"/>
       <c r="C5" s="376" t="s">
         <v>62</v>
       </c>
@@ -40140,7 +40132,7 @@
       <c r="N5" s="378"/>
     </row>
     <row r="6" spans="1:14" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B6" s="696"/>
+      <c r="B6" s="695"/>
       <c r="C6" s="379" t="s">
         <v>280</v>
       </c>
@@ -40201,16 +40193,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="697" t="s">
+      <c r="A1" s="696" t="s">
         <v>138</v>
       </c>
-      <c r="B1" s="698"/>
-      <c r="C1" s="699"/>
-      <c r="D1" s="700" t="s">
+      <c r="B1" s="697"/>
+      <c r="C1" s="698"/>
+      <c r="D1" s="699" t="s">
         <v>292</v>
       </c>
-      <c r="E1" s="700"/>
-      <c r="F1" s="701"/>
+      <c r="E1" s="699"/>
+      <c r="F1" s="700"/>
       <c r="G1" s="389" t="s">
         <v>293</v>
       </c>
@@ -40218,7 +40210,7 @@
       <c r="I1" s="461"/>
       <c r="J1" s="461"/>
       <c r="K1" s="390"/>
-      <c r="L1" s="702" t="s">
+      <c r="L1" s="701" t="s">
         <v>294</v>
       </c>
     </row>
@@ -40256,7 +40248,7 @@
       <c r="K2" s="399" t="s">
         <v>298</v>
       </c>
-      <c r="L2" s="703"/>
+      <c r="L2" s="702"/>
     </row>
     <row r="3" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="400"/>
@@ -40264,19 +40256,19 @@
       <c r="C3" s="402" t="s">
         <v>123</v>
       </c>
-      <c r="D3" s="704" t="s">
+      <c r="D3" s="703" t="s">
         <v>299</v>
       </c>
-      <c r="E3" s="705"/>
-      <c r="F3" s="706"/>
-      <c r="G3" s="707" t="s">
+      <c r="E3" s="704"/>
+      <c r="F3" s="705"/>
+      <c r="G3" s="706" t="s">
         <v>299</v>
       </c>
-      <c r="H3" s="708"/>
-      <c r="I3" s="708"/>
-      <c r="J3" s="708"/>
-      <c r="K3" s="709"/>
-      <c r="L3" s="703"/>
+      <c r="H3" s="707"/>
+      <c r="I3" s="707"/>
+      <c r="J3" s="707"/>
+      <c r="K3" s="708"/>
+      <c r="L3" s="702"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="462"/>
@@ -40329,23 +40321,23 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:29" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="630" t="s">
+      <c r="A1" s="600" t="s">
         <v>300</v>
       </c>
-      <c r="B1" s="631"/>
-      <c r="C1" s="631"/>
-      <c r="D1" s="631"/>
+      <c r="B1" s="601"/>
+      <c r="C1" s="601"/>
+      <c r="D1" s="601"/>
       <c r="E1" s="403"/>
-      <c r="F1" s="715" t="s">
+      <c r="F1" s="714" t="s">
         <v>143</v>
       </c>
-      <c r="G1" s="716"/>
-      <c r="H1" s="716"/>
+      <c r="G1" s="715"/>
+      <c r="H1" s="715"/>
       <c r="I1" s="404"/>
       <c r="J1" s="405"/>
       <c r="K1" s="404"/>
       <c r="L1" s="406"/>
-      <c r="M1" s="710" t="s">
+      <c r="M1" s="709" t="s">
         <v>301</v>
       </c>
       <c r="N1" s="407"/>
@@ -40357,19 +40349,19 @@
       <c r="R1" s="405"/>
       <c r="S1" s="404"/>
       <c r="T1" s="406"/>
-      <c r="U1" s="710" t="s">
+      <c r="U1" s="709" t="s">
         <v>303</v>
       </c>
       <c r="V1" s="407"/>
-      <c r="W1" s="717" t="s">
+      <c r="W1" s="716" t="s">
         <v>304</v>
       </c>
-      <c r="X1" s="717"/>
-      <c r="Y1" s="717"/>
-      <c r="Z1" s="717"/>
-      <c r="AA1" s="717"/>
-      <c r="AB1" s="718"/>
-      <c r="AC1" s="710" t="s">
+      <c r="X1" s="716"/>
+      <c r="Y1" s="716"/>
+      <c r="Z1" s="716"/>
+      <c r="AA1" s="716"/>
+      <c r="AB1" s="717"/>
+      <c r="AC1" s="709" t="s">
         <v>305</v>
       </c>
     </row>
@@ -40383,52 +40375,52 @@
       <c r="C2" s="409" t="s">
         <v>307</v>
       </c>
-      <c r="D2" s="712" t="s">
+      <c r="D2" s="711" t="s">
         <v>308</v>
       </c>
-      <c r="E2" s="712"/>
+      <c r="E2" s="711"/>
       <c r="F2" s="410"/>
-      <c r="G2" s="713" t="s">
+      <c r="G2" s="712" t="s">
         <v>164</v>
       </c>
-      <c r="H2" s="713"/>
-      <c r="I2" s="713" t="s">
+      <c r="H2" s="712"/>
+      <c r="I2" s="712" t="s">
         <v>165</v>
       </c>
-      <c r="J2" s="713"/>
-      <c r="K2" s="713" t="s">
+      <c r="J2" s="712"/>
+      <c r="K2" s="712" t="s">
         <v>166</v>
       </c>
-      <c r="L2" s="714"/>
-      <c r="M2" s="711"/>
+      <c r="L2" s="713"/>
+      <c r="M2" s="710"/>
       <c r="N2" s="411"/>
-      <c r="O2" s="713" t="s">
+      <c r="O2" s="712" t="s">
         <v>164</v>
       </c>
-      <c r="P2" s="713"/>
-      <c r="Q2" s="713" t="s">
+      <c r="P2" s="712"/>
+      <c r="Q2" s="712" t="s">
         <v>165</v>
       </c>
-      <c r="R2" s="713"/>
-      <c r="S2" s="713" t="s">
+      <c r="R2" s="712"/>
+      <c r="S2" s="712" t="s">
         <v>166</v>
       </c>
-      <c r="T2" s="714"/>
-      <c r="U2" s="711"/>
+      <c r="T2" s="713"/>
+      <c r="U2" s="710"/>
       <c r="V2" s="411"/>
-      <c r="W2" s="713" t="s">
+      <c r="W2" s="712" t="s">
         <v>164</v>
       </c>
-      <c r="X2" s="713"/>
-      <c r="Y2" s="713" t="s">
+      <c r="X2" s="712"/>
+      <c r="Y2" s="712" t="s">
         <v>165</v>
       </c>
-      <c r="Z2" s="713"/>
-      <c r="AA2" s="713" t="s">
+      <c r="Z2" s="712"/>
+      <c r="AA2" s="712" t="s">
         <v>166</v>
       </c>
-      <c r="AB2" s="714"/>
-      <c r="AC2" s="711"/>
+      <c r="AB2" s="713"/>
+      <c r="AC2" s="710"/>
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" s="28" t="s">

</xml_diff>